<commit_message>
added temprecord calibration august 2022 with ts2500
</commit_message>
<xml_diff>
--- a/datacombined LH001004.xls.xlsx
+++ b/datacombined LH001004.xls.xlsx
@@ -1063,25 +1063,25 @@
         <v>0.000701691937547213</v>
       </c>
       <c r="BW2" t="n">
-        <v>61</v>
+        <v>58.5</v>
       </c>
       <c r="BX2" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY2" s="2" t="n">
         <v>44757.8021180787</v>
       </c>
       <c r="BZ2" t="n">
-        <v>20.202</v>
+        <v>20.204</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.008366600265340666</v>
+        <v>0.008432740427115721</v>
       </c>
       <c r="CB2" t="n">
-        <v>14.412</v>
+        <v>14.437</v>
       </c>
       <c r="CC2" t="n">
-        <v>0.01788854381999814</v>
+        <v>0.03860051813123731</v>
       </c>
     </row>
     <row r="3">
@@ -1308,25 +1308,25 @@
         <v>0.0146597556099978</v>
       </c>
       <c r="BW3" t="n">
-        <v>79</v>
+        <v>76.5</v>
       </c>
       <c r="BX3" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY3" s="2" t="n">
         <v>44757.8646180787</v>
       </c>
       <c r="BZ3" t="n">
-        <v>20.178</v>
+        <v>20.177</v>
       </c>
       <c r="CA3" t="n">
-        <v>0.008366600265340364</v>
+        <v>0.006749485577104566</v>
       </c>
       <c r="CB3" t="n">
-        <v>32.036</v>
+        <v>31.991</v>
       </c>
       <c r="CC3" t="n">
-        <v>0.02190890230020707</v>
+        <v>0.05801340841181289</v>
       </c>
     </row>
     <row r="4">
@@ -1553,25 +1553,25 @@
         <v>0.0157839550357323</v>
       </c>
       <c r="BW4" t="n">
-        <v>97</v>
+        <v>94.5</v>
       </c>
       <c r="BX4" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY4" s="2" t="n">
         <v>44757.9271180787</v>
       </c>
       <c r="BZ4" t="n">
-        <v>20.184</v>
+        <v>20.187</v>
       </c>
       <c r="CA4" t="n">
-        <v>0.005477225575053031</v>
+        <v>0.006749485577106412</v>
       </c>
       <c r="CB4" t="n">
-        <v>47.734</v>
+        <v>47.677</v>
       </c>
       <c r="CC4" t="n">
-        <v>0.02509980079602375</v>
+        <v>0.0764562329411749</v>
       </c>
     </row>
     <row r="5">
@@ -1798,10 +1798,10 @@
         <v>0.0277421896946578</v>
       </c>
       <c r="BW5" t="n">
-        <v>115</v>
+        <v>112.5</v>
       </c>
       <c r="BX5" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY5" s="2" t="n">
         <v>44757.9896180787</v>
@@ -1810,13 +1810,13 @@
         <v>20.184</v>
       </c>
       <c r="CA5" t="n">
-        <v>0.005477225575052072</v>
+        <v>0.006992058987801609</v>
       </c>
       <c r="CB5" t="n">
-        <v>62.864</v>
+        <v>62.79599999999999</v>
       </c>
       <c r="CC5" t="n">
-        <v>0.04449719092257016</v>
+        <v>0.08461678320522562</v>
       </c>
     </row>
     <row r="6">
@@ -2043,25 +2043,25 @@
         <v>0.0271783329761665</v>
       </c>
       <c r="BW6" t="n">
-        <v>133</v>
+        <v>130.5</v>
       </c>
       <c r="BX6" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY6" s="2" t="n">
         <v>44758.0521180787</v>
       </c>
       <c r="BZ6" t="n">
-        <v>20.188</v>
+        <v>20.187</v>
       </c>
       <c r="CA6" t="n">
-        <v>0.004472135955000229</v>
+        <v>0.004830458915396513</v>
       </c>
       <c r="CB6" t="n">
-        <v>77.886</v>
+        <v>77.797</v>
       </c>
       <c r="CC6" t="n">
-        <v>0.0545893762558236</v>
+        <v>0.1120565333511122</v>
       </c>
     </row>
     <row r="7">
@@ -2288,25 +2288,25 @@
         <v>0.008463329667981681</v>
       </c>
       <c r="BW7" t="n">
-        <v>157</v>
+        <v>154.5</v>
       </c>
       <c r="BX7" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY7" s="2" t="n">
         <v>44758.13545141204</v>
       </c>
       <c r="BZ7" t="n">
-        <v>20.192</v>
+        <v>20.186</v>
       </c>
       <c r="CA7" t="n">
-        <v>0.004472135954998905</v>
+        <v>0.008432740427114602</v>
       </c>
       <c r="CB7" t="n">
-        <v>90.768</v>
+        <v>90.65400000000001</v>
       </c>
       <c r="CC7" t="n">
-        <v>0.06610597552415386</v>
+        <v>0.1380981937286352</v>
       </c>
     </row>
     <row r="8">
@@ -2533,25 +2533,25 @@
         <v>0.0280722924715457</v>
       </c>
       <c r="BW8" t="n">
-        <v>175</v>
+        <v>172.5</v>
       </c>
       <c r="BX8" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY8" s="2" t="n">
         <v>44758.19795141204</v>
       </c>
       <c r="BZ8" t="n">
-        <v>20.176</v>
+        <v>20.175</v>
       </c>
       <c r="CA8" t="n">
-        <v>0.00547722557505041</v>
+        <v>0.009718253158076227</v>
       </c>
       <c r="CB8" t="n">
-        <v>79.246</v>
+        <v>79.297</v>
       </c>
       <c r="CC8" t="n">
-        <v>0.03286335345031122</v>
+        <v>0.07024560089033939</v>
       </c>
     </row>
     <row r="9">
@@ -2778,25 +2778,25 @@
         <v>0.0225733132274093</v>
       </c>
       <c r="BW9" t="n">
-        <v>193</v>
+        <v>190.5</v>
       </c>
       <c r="BX9" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY9" s="2" t="n">
         <v>44758.26045141204</v>
       </c>
       <c r="BZ9" t="n">
-        <v>20.176</v>
+        <v>20.166</v>
       </c>
       <c r="CA9" t="n">
-        <v>0.008944271909997463</v>
+        <v>0.01349897115420986</v>
       </c>
       <c r="CB9" t="n">
-        <v>64.236</v>
+        <v>64.31800000000001</v>
       </c>
       <c r="CC9" t="n">
-        <v>0.03911521443121738</v>
+        <v>0.1036875648817737</v>
       </c>
     </row>
     <row r="10">
@@ -3023,25 +3023,25 @@
         <v>0.0225429755717043</v>
       </c>
       <c r="BW10" t="n">
-        <v>212</v>
+        <v>209.5</v>
       </c>
       <c r="BX10" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY10" s="2" t="n">
         <v>44758.32642363426</v>
       </c>
       <c r="BZ10" t="n">
-        <v>20.168</v>
+        <v>20.162</v>
       </c>
       <c r="CA10" t="n">
-        <v>0.00447213595500056</v>
+        <v>0.009189365834726952</v>
       </c>
       <c r="CB10" t="n">
-        <v>48.89</v>
+        <v>48.947</v>
       </c>
       <c r="CC10" t="n">
-        <v>0.05385164807134385</v>
+        <v>0.07572611467944226</v>
       </c>
     </row>
     <row r="11">
@@ -3268,25 +3268,25 @@
         <v>0.008418171453228349</v>
       </c>
       <c r="BW11" t="n">
-        <v>230</v>
+        <v>227.5</v>
       </c>
       <c r="BX11" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY11" s="2" t="n">
         <v>44758.38892363426</v>
       </c>
       <c r="BZ11" t="n">
-        <v>20.17</v>
+        <v>20.167</v>
       </c>
       <c r="CA11" t="n">
-        <v>0.01000000000000038</v>
+        <v>0.008232726023485489</v>
       </c>
       <c r="CB11" t="n">
-        <v>32.962</v>
+        <v>33.051</v>
       </c>
       <c r="CC11" t="n">
-        <v>0.05215361924162049</v>
+        <v>0.1047165486232018</v>
       </c>
     </row>
     <row r="12">
@@ -3513,25 +3513,25 @@
         <v>0.000755041806649868</v>
       </c>
       <c r="BW12" t="n">
-        <v>248</v>
+        <v>245.5</v>
       </c>
       <c r="BX12" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY12" s="2" t="n">
         <v>44758.45142363426</v>
       </c>
       <c r="BZ12" t="n">
-        <v>20.2</v>
+        <v>20.199</v>
       </c>
       <c r="CA12" t="n">
-        <v>0.007071067811866057</v>
+        <v>0.007378647873724963</v>
       </c>
       <c r="CB12" t="n">
-        <v>14.754</v>
+        <v>14.826</v>
       </c>
       <c r="CC12" t="n">
-        <v>0.03577708763999596</v>
+        <v>0.0888444333277737</v>
       </c>
     </row>
     <row r="13">
@@ -3758,25 +3758,25 @@
         <v>0.00266802352742819</v>
       </c>
       <c r="BW13" t="n">
-        <v>285</v>
+        <v>282.5</v>
       </c>
       <c r="BX13" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY13" s="2" t="n">
         <v>44758.57989585648</v>
       </c>
       <c r="BZ13" t="n">
-        <v>0.31</v>
+        <v>0.314</v>
       </c>
       <c r="CA13" t="n">
-        <v>0</v>
+        <v>0.0126491106406735</v>
       </c>
       <c r="CB13" t="n">
-        <v>14.038</v>
+        <v>14.035</v>
       </c>
       <c r="CC13" t="n">
-        <v>0.004472135954999286</v>
+        <v>0.01269295517643961</v>
       </c>
     </row>
     <row r="14">
@@ -4003,25 +4003,25 @@
         <v>0.015905407352011</v>
       </c>
       <c r="BW14" t="n">
-        <v>303</v>
+        <v>300.5</v>
       </c>
       <c r="BX14" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY14" s="2" t="n">
         <v>44758.64239585648</v>
       </c>
       <c r="BZ14" t="n">
-        <v>0.264</v>
+        <v>0.27</v>
       </c>
       <c r="CA14" t="n">
-        <v>0.005477225575051667</v>
+        <v>0.01154700538379252</v>
       </c>
       <c r="CB14" t="n">
-        <v>31.4</v>
+        <v>31.297</v>
       </c>
       <c r="CC14" t="n">
-        <v>0.06745368781616265</v>
+        <v>0.1238323239079546</v>
       </c>
     </row>
     <row r="15">
@@ -4248,25 +4248,25 @@
         <v>0.0194379026605417</v>
       </c>
       <c r="BW15" t="n">
-        <v>321</v>
+        <v>318.5</v>
       </c>
       <c r="BX15" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY15" s="2" t="n">
         <v>44758.70489585648</v>
       </c>
       <c r="BZ15" t="n">
-        <v>0.264</v>
+        <v>0.265</v>
       </c>
       <c r="CA15" t="n">
-        <v>0.005477225575051669</v>
+        <v>0.005270462766947304</v>
       </c>
       <c r="CB15" t="n">
-        <v>47.09</v>
+        <v>46.98400000000001</v>
       </c>
       <c r="CC15" t="n">
-        <v>0.05787918451395142</v>
+        <v>0.1327654573549426</v>
       </c>
     </row>
     <row r="16">
@@ -4493,10 +4493,10 @@
         <v>0.0251903516332451</v>
       </c>
       <c r="BW16" t="n">
-        <v>339</v>
+        <v>336.5</v>
       </c>
       <c r="BX16" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY16" s="2" t="n">
         <v>44758.76739585648</v>
@@ -4505,13 +4505,13 @@
         <v>0.264</v>
       </c>
       <c r="CA16" t="n">
-        <v>0.00547722557505166</v>
+        <v>0.005163977794943231</v>
       </c>
       <c r="CB16" t="n">
-        <v>62.414</v>
+        <v>62.29200000000001</v>
       </c>
       <c r="CC16" t="n">
-        <v>0.07162401831787898</v>
+        <v>0.1483838865166202</v>
       </c>
     </row>
     <row r="17">
@@ -4738,25 +4738,25 @@
         <v>0.0377494533180363</v>
       </c>
       <c r="BW17" t="n">
-        <v>357</v>
+        <v>354.5</v>
       </c>
       <c r="BX17" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY17" s="2" t="n">
         <v>44758.82989585648</v>
       </c>
       <c r="BZ17" t="n">
-        <v>0.262</v>
+        <v>0.275</v>
       </c>
       <c r="CA17" t="n">
-        <v>0.004472135954999588</v>
+        <v>0.0177951304200522</v>
       </c>
       <c r="CB17" t="n">
-        <v>77.678</v>
+        <v>77.51500000000001</v>
       </c>
       <c r="CC17" t="n">
-        <v>0.08288546314041735</v>
+        <v>0.1989556064385578</v>
       </c>
     </row>
     <row r="18">
@@ -4983,10 +4983,10 @@
         <v>0.00919625607684167</v>
       </c>
       <c r="BW18" t="n">
-        <v>387</v>
+        <v>384.5</v>
       </c>
       <c r="BX18" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY18" s="2" t="n">
         <v>44758.93406252315</v>
@@ -4998,10 +4998,10 @@
         <v>0</v>
       </c>
       <c r="CB18" t="n">
-        <v>93.73000000000002</v>
+        <v>93.56699999999999</v>
       </c>
       <c r="CC18" t="n">
-        <v>0.09027735042632433</v>
+        <v>0.194995726448902</v>
       </c>
     </row>
     <row r="19">
@@ -5228,10 +5228,10 @@
         <v>0.0446562039041779</v>
       </c>
       <c r="BW19" t="n">
-        <v>406</v>
+        <v>403.5</v>
       </c>
       <c r="BX19" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY19" s="2" t="n">
         <v>44759.00003474537</v>
@@ -5243,10 +5243,10 @@
         <v>0</v>
       </c>
       <c r="CB19" t="n">
-        <v>80.114</v>
+        <v>80.224</v>
       </c>
       <c r="CC19" t="n">
-        <v>0.04277849927241382</v>
+        <v>0.13777598565142</v>
       </c>
     </row>
     <row r="20">
@@ -5473,25 +5473,25 @@
         <v>0.0295955860367739</v>
       </c>
       <c r="BW20" t="n">
-        <v>424</v>
+        <v>421.5</v>
       </c>
       <c r="BX20" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY20" s="2" t="n">
         <v>44759.06253474537</v>
       </c>
       <c r="BZ20" t="n">
-        <v>0.26</v>
+        <v>0.2480000000000001</v>
       </c>
       <c r="CA20" t="n">
-        <v>0</v>
+        <v>0.01549193338482966</v>
       </c>
       <c r="CB20" t="n">
-        <v>64.87</v>
+        <v>64.99099999999999</v>
       </c>
       <c r="CC20" t="n">
-        <v>0.06082762530299141</v>
+        <v>0.1490301982821035</v>
       </c>
     </row>
     <row r="21">
@@ -5718,10 +5718,10 @@
         <v>0.0201627265883991</v>
       </c>
       <c r="BW21" t="n">
-        <v>442</v>
+        <v>439.5</v>
       </c>
       <c r="BX21" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY21" s="2" t="n">
         <v>44759.12503474537</v>
@@ -5733,10 +5733,10 @@
         <v>0</v>
       </c>
       <c r="CB21" t="n">
-        <v>49.218</v>
+        <v>49.346</v>
       </c>
       <c r="CC21" t="n">
-        <v>0.05718391382198185</v>
+        <v>0.1580576547409912</v>
       </c>
     </row>
     <row r="22">
@@ -5963,10 +5963,10 @@
         <v>0.00842360566902655</v>
       </c>
       <c r="BW22" t="n">
-        <v>461</v>
+        <v>458.5</v>
       </c>
       <c r="BX22" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY22" s="2" t="n">
         <v>44759.19100696759</v>
@@ -5978,10 +5978,10 @@
         <v>0</v>
       </c>
       <c r="CB22" t="n">
-        <v>33.11</v>
+        <v>33.205</v>
       </c>
       <c r="CC22" t="n">
-        <v>0.0587367006223555</v>
+        <v>0.1204851304795224</v>
       </c>
     </row>
     <row r="23">
@@ -6208,10 +6208,10 @@
         <v>0.00152499135736525</v>
       </c>
       <c r="BW23" t="n">
-        <v>479</v>
+        <v>476.5</v>
       </c>
       <c r="BX23" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY23" s="2" t="n">
         <v>44759.25350696759</v>
@@ -6223,10 +6223,10 @@
         <v>0</v>
       </c>
       <c r="CB23" t="n">
-        <v>15.136</v>
+        <v>15.272</v>
       </c>
       <c r="CC23" t="n">
-        <v>0.08848728722251629</v>
+        <v>0.1710620420263421</v>
       </c>
     </row>
     <row r="24">
@@ -6453,25 +6453,25 @@
         <v>0.0021770732213712</v>
       </c>
       <c r="BW24" t="n">
-        <v>515</v>
+        <v>512.5</v>
       </c>
       <c r="BX24" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY24" s="2" t="n">
         <v>44759.37850696759</v>
       </c>
       <c r="BZ24" t="n">
-        <v>10.128</v>
+        <v>10.117</v>
       </c>
       <c r="CA24" t="n">
-        <v>0.004472135955000179</v>
+        <v>0.01418136492412219</v>
       </c>
       <c r="CB24" t="n">
-        <v>14.598</v>
+        <v>14.626</v>
       </c>
       <c r="CC24" t="n">
-        <v>0.01788854381999826</v>
+        <v>0.03502380143083626</v>
       </c>
     </row>
     <row r="25">
@@ -6698,25 +6698,25 @@
         <v>0.01517354399697</v>
       </c>
       <c r="BW25" t="n">
-        <v>533</v>
+        <v>530.5</v>
       </c>
       <c r="BX25" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY25" s="2" t="n">
         <v>44759.44100696759</v>
       </c>
       <c r="BZ25" t="n">
-        <v>10.14</v>
+        <v>10.139</v>
       </c>
       <c r="CA25" t="n">
-        <v>0</v>
+        <v>0.003162277660168043</v>
       </c>
       <c r="CB25" t="n">
-        <v>32.16</v>
+        <v>32.112</v>
       </c>
       <c r="CC25" t="n">
-        <v>0.04123105625617637</v>
+        <v>0.06511528238439848</v>
       </c>
     </row>
     <row r="26">
@@ -6943,25 +6943,25 @@
         <v>0.0209224681038087</v>
       </c>
       <c r="BW26" t="n">
-        <v>551</v>
+        <v>548.5</v>
       </c>
       <c r="BX26" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY26" s="2" t="n">
         <v>44759.50350696759</v>
       </c>
       <c r="BZ26" t="n">
-        <v>10.17</v>
+        <v>10.172</v>
       </c>
       <c r="CA26" t="n">
-        <v>0</v>
+        <v>0.006324555320336562</v>
       </c>
       <c r="CB26" t="n">
-        <v>47.78400000000001</v>
+        <v>47.70399999999999</v>
       </c>
       <c r="CC26" t="n">
-        <v>0.04827007354458922</v>
+        <v>0.09890511727015104</v>
       </c>
     </row>
     <row r="27">
@@ -7188,25 +7188,25 @@
         <v>0.0237688290448408</v>
       </c>
       <c r="BW27" t="n">
-        <v>570</v>
+        <v>567.5</v>
       </c>
       <c r="BX27" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY27" s="2" t="n">
         <v>44759.56947918981</v>
       </c>
       <c r="BZ27" t="n">
-        <v>10.17</v>
+        <v>10.172</v>
       </c>
       <c r="CA27" t="n">
-        <v>0</v>
+        <v>0.006324555320336562</v>
       </c>
       <c r="CB27" t="n">
-        <v>63.036</v>
+        <v>62.961</v>
       </c>
       <c r="CC27" t="n">
-        <v>0.037815340802381</v>
+        <v>0.0882483868281875</v>
       </c>
     </row>
     <row r="28">
@@ -7433,25 +7433,25 @@
         <v>0.0338806430453412</v>
       </c>
       <c r="BW28" t="n">
-        <v>588</v>
+        <v>585.5</v>
       </c>
       <c r="BX28" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY28" s="2" t="n">
         <v>44759.63197918981</v>
       </c>
       <c r="BZ28" t="n">
-        <v>10.18</v>
+        <v>10.184</v>
       </c>
       <c r="CA28" t="n">
-        <v>0.01000000000000045</v>
+        <v>0.01173787790777219</v>
       </c>
       <c r="CB28" t="n">
-        <v>78.172</v>
+        <v>78.059</v>
       </c>
       <c r="CC28" t="n">
-        <v>0.05718391382198115</v>
+        <v>0.1403527302509239</v>
       </c>
     </row>
     <row r="29">
@@ -7678,25 +7678,25 @@
         <v>0.00899328417015822</v>
       </c>
       <c r="BW29" t="n">
-        <v>612</v>
+        <v>609.5</v>
       </c>
       <c r="BX29" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY29" s="2" t="n">
         <v>44759.71531252315</v>
       </c>
       <c r="BZ29" t="n">
-        <v>10.182</v>
+        <v>10.183</v>
       </c>
       <c r="CA29" t="n">
-        <v>0.01095445115010316</v>
+        <v>0.009486832980504841</v>
       </c>
       <c r="CB29" t="n">
-        <v>93.88800000000001</v>
+        <v>93.71100000000001</v>
       </c>
       <c r="CC29" t="n">
-        <v>0.09628083921528824</v>
+        <v>0.2138769116415681</v>
       </c>
     </row>
     <row r="30">
@@ -7923,25 +7923,25 @@
         <v>0.0225116762022843</v>
       </c>
       <c r="BW30" t="n">
-        <v>631</v>
+        <v>628.5</v>
       </c>
       <c r="BX30" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY30" s="2" t="n">
         <v>44759.78128474537</v>
       </c>
       <c r="BZ30" t="n">
-        <v>10.17</v>
+        <v>10.168</v>
       </c>
       <c r="CA30" t="n">
-        <v>0</v>
+        <v>0.006324555320336323</v>
       </c>
       <c r="CB30" t="n">
-        <v>79.83000000000001</v>
+        <v>79.90899999999999</v>
       </c>
       <c r="CC30" t="n">
-        <v>0.03082207001484643</v>
+        <v>0.09757618106438955</v>
       </c>
     </row>
     <row r="31">
@@ -8168,10 +8168,10 @@
         <v>0.0302800114966396</v>
       </c>
       <c r="BW31" t="n">
-        <v>649</v>
+        <v>646.5</v>
       </c>
       <c r="BX31" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY31" s="2" t="n">
         <v>44759.84378474537</v>
@@ -8183,10 +8183,10 @@
         <v>0</v>
       </c>
       <c r="CB31" t="n">
-        <v>64.61799999999999</v>
+        <v>64.70599999999999</v>
       </c>
       <c r="CC31" t="n">
-        <v>0.03633180424917193</v>
+        <v>0.1199259030494343</v>
       </c>
     </row>
     <row r="32">
@@ -8413,10 +8413,10 @@
         <v>0.021881126095143</v>
       </c>
       <c r="BW32" t="n">
-        <v>667</v>
+        <v>664.5</v>
       </c>
       <c r="BX32" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY32" s="2" t="n">
         <v>44759.90628474537</v>
@@ -8428,10 +8428,10 @@
         <v>0</v>
       </c>
       <c r="CB32" t="n">
-        <v>49.106</v>
+        <v>49.199</v>
       </c>
       <c r="CC32" t="n">
-        <v>0.03286335345031081</v>
+        <v>0.1345321109954386</v>
       </c>
     </row>
     <row r="33">
@@ -8658,25 +8658,25 @@
         <v>0.008287300040558479</v>
       </c>
       <c r="BW33" t="n">
-        <v>685</v>
+        <v>682.5</v>
       </c>
       <c r="BX33" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY33" s="2" t="n">
         <v>44759.96878474537</v>
       </c>
       <c r="BZ33" t="n">
-        <v>10.178</v>
+        <v>10.174</v>
       </c>
       <c r="CA33" t="n">
-        <v>0.01095445115010258</v>
+        <v>0.008432740427115447</v>
       </c>
       <c r="CB33" t="n">
-        <v>33.056</v>
+        <v>33.15300000000001</v>
       </c>
       <c r="CC33" t="n">
-        <v>0.04827007354458875</v>
+        <v>0.1139249265476579</v>
       </c>
     </row>
     <row r="34">
@@ -8903,25 +8903,25 @@
         <v>0.00146911129708374</v>
       </c>
       <c r="BW34" t="n">
-        <v>703</v>
+        <v>700.5</v>
       </c>
       <c r="BX34" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY34" s="2" t="n">
         <v>44760.03128474537</v>
       </c>
       <c r="BZ34" t="n">
-        <v>10.21</v>
+        <v>10.208</v>
       </c>
       <c r="CA34" t="n">
-        <v>0</v>
+        <v>0.00632455532033739</v>
       </c>
       <c r="CB34" t="n">
-        <v>14.932</v>
+        <v>15.045</v>
       </c>
       <c r="CC34" t="n">
-        <v>0.05215361924162091</v>
+        <v>0.1419115530493865</v>
       </c>
     </row>
     <row r="35">
@@ -9148,25 +9148,25 @@
         <v>0.00107149185068248</v>
       </c>
       <c r="BW35" t="n">
-        <v>740</v>
+        <v>737.5</v>
       </c>
       <c r="BX35" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY35" s="2" t="n">
         <v>44760.15975696759</v>
       </c>
       <c r="BZ35" t="n">
-        <v>20.204</v>
+        <v>20.201</v>
       </c>
       <c r="CA35" t="n">
-        <v>0.01140175425099067</v>
+        <v>0.008755950357709204</v>
       </c>
       <c r="CB35" t="n">
-        <v>14.42</v>
+        <v>14.453</v>
       </c>
       <c r="CC35" t="n">
-        <v>0</v>
+        <v>0.04498147766951898</v>
       </c>
     </row>
     <row r="36">
@@ -9393,10 +9393,10 @@
         <v>0.0167744384150581</v>
       </c>
       <c r="BW36" t="n">
-        <v>758</v>
+        <v>755.5</v>
       </c>
       <c r="BX36" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY36" s="2" t="n">
         <v>44760.22225696759</v>
@@ -9405,13 +9405,13 @@
         <v>20.188</v>
       </c>
       <c r="CA36" t="n">
-        <v>0.01303840481040577</v>
+        <v>0.01229272594305779</v>
       </c>
       <c r="CB36" t="n">
-        <v>31.966</v>
+        <v>31.915</v>
       </c>
       <c r="CC36" t="n">
-        <v>0.02190890230020516</v>
+        <v>0.0604152298679721</v>
       </c>
     </row>
     <row r="37">
@@ -9638,25 +9638,25 @@
         <v>0.0181263629069722</v>
       </c>
       <c r="BW37" t="n">
-        <v>776</v>
+        <v>773.5</v>
       </c>
       <c r="BX37" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY37" s="2" t="n">
         <v>44760.28475696759</v>
       </c>
       <c r="BZ37" t="n">
-        <v>20.17</v>
+        <v>20.178</v>
       </c>
       <c r="CA37" t="n">
-        <v>0.007071067811865795</v>
+        <v>0.01135292424394991</v>
       </c>
       <c r="CB37" t="n">
-        <v>47.70800000000001</v>
+        <v>47.66199999999999</v>
       </c>
       <c r="CC37" t="n">
-        <v>0.02489979919597755</v>
+        <v>0.07161626134397922</v>
       </c>
     </row>
     <row r="38">
@@ -9883,25 +9883,25 @@
         <v>0.0176444642855451</v>
       </c>
       <c r="BW38" t="n">
-        <v>794</v>
+        <v>791.5</v>
       </c>
       <c r="BX38" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY38" s="2" t="n">
         <v>44760.34725696759</v>
       </c>
       <c r="BZ38" t="n">
-        <v>20.176</v>
+        <v>20.18</v>
       </c>
       <c r="CA38" t="n">
-        <v>0.00547722557505041</v>
+        <v>0.01054092553389393</v>
       </c>
       <c r="CB38" t="n">
-        <v>62.98</v>
+        <v>62.923</v>
       </c>
       <c r="CC38" t="n">
-        <v>0.04062019202318265</v>
+        <v>0.07513691207094231</v>
       </c>
     </row>
     <row r="39">
@@ -10128,25 +10128,25 @@
         <v>0.0192728560181386</v>
       </c>
       <c r="BW39" t="n">
-        <v>812</v>
+        <v>809.5</v>
       </c>
       <c r="BX39" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY39" s="2" t="n">
         <v>44760.40975696759</v>
       </c>
       <c r="BZ39" t="n">
-        <v>20.176</v>
+        <v>20.179</v>
       </c>
       <c r="CA39" t="n">
-        <v>0.008944271910000284</v>
+        <v>0.009944289260117499</v>
       </c>
       <c r="CB39" t="n">
-        <v>78.146</v>
+        <v>78.05299999999998</v>
       </c>
       <c r="CC39" t="n">
-        <v>0.04929503017546359</v>
+        <v>0.1166238016492028</v>
       </c>
     </row>
     <row r="40">
@@ -10373,25 +10373,25 @@
         <v>0.009571330948875431</v>
       </c>
       <c r="BW40" t="n">
-        <v>848</v>
+        <v>845.5</v>
       </c>
       <c r="BX40" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY40" s="2" t="n">
         <v>44760.53475696759</v>
       </c>
       <c r="BZ40" t="n">
-        <v>20.178</v>
+        <v>20.179</v>
       </c>
       <c r="CA40" t="n">
-        <v>0.01095445115010232</v>
+        <v>0.009944289260117341</v>
       </c>
       <c r="CB40" t="n">
-        <v>91.444</v>
+        <v>91.39400000000001</v>
       </c>
       <c r="CC40" t="n">
-        <v>0.02509980079602173</v>
+        <v>0.06022181221672326</v>
       </c>
     </row>
     <row r="41">
@@ -10618,25 +10618,25 @@
         <v>0.0242326448097438</v>
       </c>
       <c r="BW41" t="n">
-        <v>867</v>
+        <v>864.5</v>
       </c>
       <c r="BX41" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY41" s="2" t="n">
         <v>44760.60072918981</v>
       </c>
       <c r="BZ41" t="n">
-        <v>20.162</v>
+        <v>20.159</v>
       </c>
       <c r="CA41" t="n">
-        <v>0.004472135954999898</v>
+        <v>0.01100504934614711</v>
       </c>
       <c r="CB41" t="n">
-        <v>79.684</v>
+        <v>79.74399999999999</v>
       </c>
       <c r="CC41" t="n">
-        <v>0.0250998007960218</v>
+        <v>0.07647802879839503</v>
       </c>
     </row>
     <row r="42">
@@ -10863,25 +10863,25 @@
         <v>0.0289670432782256</v>
       </c>
       <c r="BW42" t="n">
-        <v>885</v>
+        <v>882.5</v>
       </c>
       <c r="BX42" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY42" s="2" t="n">
         <v>44760.66322918981</v>
       </c>
       <c r="BZ42" t="n">
-        <v>20.168</v>
+        <v>20.164</v>
       </c>
       <c r="CA42" t="n">
-        <v>0.01095445115010303</v>
+        <v>0.01173787790777304</v>
       </c>
       <c r="CB42" t="n">
-        <v>64.46599999999999</v>
+        <v>64.55199999999999</v>
       </c>
       <c r="CC42" t="n">
-        <v>0.03911521443120893</v>
+        <v>0.1094227276818325</v>
       </c>
     </row>
     <row r="43">
@@ -11108,25 +11108,25 @@
         <v>0.0144204945712011</v>
       </c>
       <c r="BW43" t="n">
-        <v>903</v>
+        <v>900.5</v>
       </c>
       <c r="BX43" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY43" s="2" t="n">
         <v>44760.72572918981</v>
       </c>
       <c r="BZ43" t="n">
-        <v>20.168</v>
+        <v>20.169</v>
       </c>
       <c r="CA43" t="n">
-        <v>0.008366600265341603</v>
+        <v>0.00994428926011854</v>
       </c>
       <c r="CB43" t="n">
-        <v>48.876</v>
+        <v>48.957</v>
       </c>
       <c r="CC43" t="n">
-        <v>0.03781534080237762</v>
+        <v>0.1029616973010382</v>
       </c>
     </row>
     <row r="44">
@@ -11353,25 +11353,25 @@
         <v>0.00503138393063652</v>
       </c>
       <c r="BW44" t="n">
-        <v>922</v>
+        <v>919.5</v>
       </c>
       <c r="BX44" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY44" s="2" t="n">
         <v>44760.79170141204</v>
       </c>
       <c r="BZ44" t="n">
-        <v>20.17</v>
+        <v>20.17299999999999</v>
       </c>
       <c r="CA44" t="n">
-        <v>0.01224744871391684</v>
+        <v>0.01251665557034631</v>
       </c>
       <c r="CB44" t="n">
-        <v>32.818</v>
+        <v>32.902</v>
       </c>
       <c r="CC44" t="n">
-        <v>0.03346640106135983</v>
+        <v>0.1067499674733263</v>
       </c>
     </row>
     <row r="45">
@@ -11598,25 +11598,25 @@
         <v>0.000831330744235239</v>
       </c>
       <c r="BW45" t="n">
-        <v>940</v>
+        <v>937.5</v>
       </c>
       <c r="BX45" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY45" s="2" t="n">
         <v>44760.85420141204</v>
       </c>
       <c r="BZ45" t="n">
-        <v>20.196</v>
+        <v>20.198</v>
       </c>
       <c r="CA45" t="n">
-        <v>0.008944271909999597</v>
+        <v>0.0103279555898857</v>
       </c>
       <c r="CB45" t="n">
-        <v>14.69</v>
+        <v>14.762</v>
       </c>
       <c r="CC45" t="n">
-        <v>0.03999999999999963</v>
+        <v>0.08804039476916811</v>
       </c>
     </row>
     <row r="46">
@@ -11843,25 +11843,25 @@
         <v>0.000646837188110678</v>
       </c>
       <c r="BW46" t="n">
-        <v>976</v>
+        <v>973.5</v>
       </c>
       <c r="BX46" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY46" s="2" t="n">
         <v>44760.97920141204</v>
       </c>
       <c r="BZ46" t="n">
-        <v>30.136</v>
+        <v>30.135</v>
       </c>
       <c r="CA46" t="n">
-        <v>0.005477225575052072</v>
+        <v>0.005270462766947552</v>
       </c>
       <c r="CB46" t="n">
-        <v>14.45</v>
+        <v>14.466</v>
       </c>
       <c r="CC46" t="n">
-        <v>0</v>
+        <v>0.02366431913239847</v>
       </c>
     </row>
     <row r="47">
@@ -12088,25 +12088,25 @@
         <v>0.00333959537278768</v>
       </c>
       <c r="BW47" t="n">
-        <v>994</v>
+        <v>991.5</v>
       </c>
       <c r="BX47" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY47" s="2" t="n">
         <v>44761.04170141204</v>
       </c>
       <c r="BZ47" t="n">
-        <v>30.108</v>
+        <v>30.113</v>
       </c>
       <c r="CA47" t="n">
-        <v>0.01643167672515601</v>
+        <v>0.01251665557034664</v>
       </c>
       <c r="CB47" t="n">
-        <v>31.88</v>
+        <v>31.853</v>
       </c>
       <c r="CC47" t="n">
-        <v>0.02236067977499782</v>
+        <v>0.0374314187696819</v>
       </c>
     </row>
     <row r="48">
@@ -12333,25 +12333,25 @@
         <v>0.00763387812485306</v>
       </c>
       <c r="BW48" t="n">
-        <v>1012</v>
+        <v>1009.5</v>
       </c>
       <c r="BX48" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY48" s="2" t="n">
         <v>44761.10420141204</v>
       </c>
       <c r="BZ48" t="n">
-        <v>30.112</v>
+        <v>30.11100000000001</v>
       </c>
       <c r="CA48" t="n">
-        <v>0.004472135955000229</v>
+        <v>0.003162277660169047</v>
       </c>
       <c r="CB48" t="n">
-        <v>47.706</v>
+        <v>47.653</v>
       </c>
       <c r="CC48" t="n">
-        <v>0.02880972058177584</v>
+        <v>0.06600505031182778</v>
       </c>
     </row>
     <row r="49">
@@ -12578,25 +12578,25 @@
         <v>0.0179911216107671</v>
       </c>
       <c r="BW49" t="n">
-        <v>1031</v>
+        <v>1028.5</v>
       </c>
       <c r="BX49" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY49" s="2" t="n">
         <v>44761.17017363426</v>
       </c>
       <c r="BZ49" t="n">
-        <v>30.108</v>
+        <v>30.109</v>
       </c>
       <c r="CA49" t="n">
-        <v>0.004472135954998905</v>
+        <v>0.003162277660167932</v>
       </c>
       <c r="CB49" t="n">
-        <v>63.126</v>
+        <v>63.078</v>
       </c>
       <c r="CC49" t="n">
-        <v>0.03911521443121669</v>
+        <v>0.06408327915038896</v>
       </c>
     </row>
     <row r="50">
@@ -12823,25 +12823,25 @@
         <v>0.0144674279942709</v>
       </c>
       <c r="BW50" t="n">
-        <v>1049</v>
+        <v>1046.5</v>
       </c>
       <c r="BX50" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY50" s="2" t="n">
         <v>44761.23267363426</v>
       </c>
       <c r="BZ50" t="n">
-        <v>30.116</v>
+        <v>30.115</v>
       </c>
       <c r="CA50" t="n">
-        <v>0.005477225575051761</v>
+        <v>0.005270462766948318</v>
       </c>
       <c r="CB50" t="n">
-        <v>78.486</v>
+        <v>78.395</v>
       </c>
       <c r="CC50" t="n">
-        <v>0.05128352561983274</v>
+        <v>0.1131616346451226</v>
       </c>
     </row>
     <row r="51">
@@ -13068,25 +13068,25 @@
         <v>0.008934849454680821</v>
       </c>
       <c r="BW51" t="n">
-        <v>1085</v>
+        <v>1082.5</v>
       </c>
       <c r="BX51" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY51" s="2" t="n">
         <v>44761.35767363426</v>
       </c>
       <c r="BZ51" t="n">
-        <v>30.11</v>
+        <v>30.10500000000001</v>
       </c>
       <c r="CA51" t="n">
-        <v>0</v>
+        <v>0.01354006400772751</v>
       </c>
       <c r="CB51" t="n">
-        <v>94.94200000000001</v>
+        <v>94.87100000000001</v>
       </c>
       <c r="CC51" t="n">
-        <v>0.04919349550500036</v>
+        <v>0.08761658899241828</v>
       </c>
     </row>
     <row r="52">
@@ -13313,25 +13313,25 @@
         <v>0.0129186255364118</v>
       </c>
       <c r="BW52" t="n">
-        <v>1103</v>
+        <v>1100.5</v>
       </c>
       <c r="BX52" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY52" s="2" t="n">
         <v>44761.42017363426</v>
       </c>
       <c r="BZ52" t="n">
-        <v>30.098</v>
+        <v>30.097</v>
       </c>
       <c r="CA52" t="n">
-        <v>0.0164316767251552</v>
+        <v>0.01494434118097356</v>
       </c>
       <c r="CB52" t="n">
-        <v>80.23399999999999</v>
+        <v>80.31500000000001</v>
       </c>
       <c r="CC52" t="n">
-        <v>0.04449719092256784</v>
+        <v>0.1001387925719998</v>
       </c>
     </row>
     <row r="53">
@@ -13558,25 +13558,25 @@
         <v>0.0150672606362789</v>
       </c>
       <c r="BW53" t="n">
-        <v>1122</v>
+        <v>1119.5</v>
       </c>
       <c r="BX53" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY53" s="2" t="n">
         <v>44761.48614585648</v>
       </c>
       <c r="BZ53" t="n">
-        <v>30.11</v>
+        <v>30.103</v>
       </c>
       <c r="CA53" t="n">
-        <v>0</v>
+        <v>0.01251665557034623</v>
       </c>
       <c r="CB53" t="n">
-        <v>64.624</v>
+        <v>64.703</v>
       </c>
       <c r="CC53" t="n">
-        <v>0.03911521443121399</v>
+        <v>0.09603818684946483</v>
       </c>
     </row>
     <row r="54">
@@ -13803,25 +13803,25 @@
         <v>0.0129115200755056</v>
       </c>
       <c r="BW54" t="n">
-        <v>1140</v>
+        <v>1137.5</v>
       </c>
       <c r="BX54" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY54" s="2" t="n">
         <v>44761.54864585648</v>
       </c>
       <c r="BZ54" t="n">
-        <v>30.092</v>
+        <v>30.09399999999999</v>
       </c>
       <c r="CA54" t="n">
-        <v>0.01643167672515581</v>
+        <v>0.01505545305418163</v>
       </c>
       <c r="CB54" t="n">
-        <v>48.824</v>
+        <v>48.89800000000001</v>
       </c>
       <c r="CC54" t="n">
-        <v>0.03507135583349842</v>
+        <v>0.0944927980794761</v>
       </c>
     </row>
     <row r="55">
@@ -14048,25 +14048,25 @@
         <v>0.00341083895750232</v>
       </c>
       <c r="BW55" t="n">
-        <v>1158</v>
+        <v>1155.5</v>
       </c>
       <c r="BX55" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY55" s="2" t="n">
         <v>44761.61114585648</v>
       </c>
       <c r="BZ55" t="n">
-        <v>30.108</v>
+        <v>30.106</v>
       </c>
       <c r="CA55" t="n">
-        <v>0.004472135954999402</v>
+        <v>0.009660917830793175</v>
       </c>
       <c r="CB55" t="n">
-        <v>32.644</v>
+        <v>32.706</v>
       </c>
       <c r="CC55" t="n">
-        <v>0.02880972058177584</v>
+        <v>0.07167829363048071</v>
       </c>
     </row>
     <row r="56">
@@ -14293,25 +14293,25 @@
         <v>0.00057488439792961</v>
       </c>
       <c r="BW56" t="n">
-        <v>1176</v>
+        <v>1173.5</v>
       </c>
       <c r="BX56" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY56" s="2" t="n">
         <v>44761.67364585648</v>
       </c>
       <c r="BZ56" t="n">
-        <v>30.116</v>
+        <v>30.115</v>
       </c>
       <c r="CA56" t="n">
-        <v>0.005477225575052072</v>
+        <v>0.005270462766948193</v>
       </c>
       <c r="CB56" t="n">
-        <v>14.616</v>
+        <v>14.667</v>
       </c>
       <c r="CC56" t="n">
-        <v>0.03714835124201311</v>
+        <v>0.06912950809089316</v>
       </c>
     </row>
     <row r="57">
@@ -14538,25 +14538,25 @@
         <v>0.000655318745442699</v>
       </c>
       <c r="BW57" t="n">
-        <v>1212</v>
+        <v>1209.5</v>
       </c>
       <c r="BX57" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY57" s="2" t="n">
         <v>44761.79864585648</v>
       </c>
       <c r="BZ57" t="n">
-        <v>40.142</v>
+        <v>40.13499999999999</v>
       </c>
       <c r="CA57" t="n">
-        <v>0.0109544511501006</v>
+        <v>0.01080123449734656</v>
       </c>
       <c r="CB57" t="n">
-        <v>14.438</v>
+        <v>14.452</v>
       </c>
       <c r="CC57" t="n">
-        <v>0.01643167672515435</v>
+        <v>0.02347575581554569</v>
       </c>
     </row>
     <row r="58">
@@ -14783,25 +14783,25 @@
         <v>0.00335584186171879</v>
       </c>
       <c r="BW58" t="n">
-        <v>1230</v>
+        <v>1227.5</v>
       </c>
       <c r="BX58" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY58" s="2" t="n">
         <v>44761.86114585648</v>
       </c>
       <c r="BZ58" t="n">
-        <v>40.112</v>
+        <v>40.108</v>
       </c>
       <c r="CA58" t="n">
-        <v>0.0109544511501006</v>
+        <v>0.01032795558988432</v>
       </c>
       <c r="CB58" t="n">
-        <v>31.72</v>
+        <v>31.692</v>
       </c>
       <c r="CC58" t="n">
-        <v>0.02236067977499987</v>
+        <v>0.03614784456460238</v>
       </c>
     </row>
     <row r="59">
@@ -15028,25 +15028,25 @@
         <v>0.0116282408980297</v>
       </c>
       <c r="BW59" t="n">
-        <v>1248</v>
+        <v>1245.5</v>
       </c>
       <c r="BX59" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY59" s="2" t="n">
         <v>44761.92364585648</v>
       </c>
       <c r="BZ59" t="n">
-        <v>40.12</v>
+        <v>40.112</v>
       </c>
       <c r="CA59" t="n">
-        <v>0</v>
+        <v>0.01032795558988444</v>
       </c>
       <c r="CB59" t="n">
-        <v>47.652</v>
+        <v>47.60999999999999</v>
       </c>
       <c r="CC59" t="n">
-        <v>0.02489979919597656</v>
+        <v>0.05456901847914816</v>
       </c>
     </row>
     <row r="60">
@@ -15273,25 +15273,25 @@
         <v>0.0121852879214425</v>
       </c>
       <c r="BW60" t="n">
-        <v>1266</v>
+        <v>1263.5</v>
       </c>
       <c r="BX60" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY60" s="2" t="n">
         <v>44761.98614585648</v>
       </c>
       <c r="BZ60" t="n">
-        <v>40.1</v>
+        <v>40.102</v>
       </c>
       <c r="CA60" t="n">
-        <v>0</v>
+        <v>0.006324555320337747</v>
       </c>
       <c r="CB60" t="n">
-        <v>63.23999999999999</v>
+        <v>63.189</v>
       </c>
       <c r="CC60" t="n">
-        <v>0.02121320343559692</v>
+        <v>0.0617251974480457</v>
       </c>
     </row>
     <row r="61">
@@ -15518,25 +15518,25 @@
         <v>0.009056120063992871</v>
       </c>
       <c r="BW61" t="n">
-        <v>1285</v>
+        <v>1282.5</v>
       </c>
       <c r="BX61" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY61" s="2" t="n">
         <v>44762.0521180787</v>
       </c>
       <c r="BZ61" t="n">
-        <v>40.112</v>
+        <v>40.11800000000001</v>
       </c>
       <c r="CA61" t="n">
-        <v>0.01095445115010082</v>
+        <v>0.01316561177208872</v>
       </c>
       <c r="CB61" t="n">
-        <v>78.88</v>
+        <v>78.80499999999999</v>
       </c>
       <c r="CC61" t="n">
-        <v>0.04743416490252749</v>
+        <v>0.09228578799937327</v>
       </c>
     </row>
     <row r="62">
@@ -15763,25 +15763,25 @@
         <v>0.00896775163315265</v>
       </c>
       <c r="BW62" t="n">
-        <v>1321</v>
+        <v>1318.5</v>
       </c>
       <c r="BX62" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY62" s="2" t="n">
         <v>44762.1771180787</v>
       </c>
       <c r="BZ62" t="n">
-        <v>40.112</v>
+        <v>40.11200000000001</v>
       </c>
       <c r="CA62" t="n">
-        <v>0.0164316767251552</v>
+        <v>0.01316561177208655</v>
       </c>
       <c r="CB62" t="n">
-        <v>95.072</v>
+        <v>95.006</v>
       </c>
       <c r="CC62" t="n">
-        <v>0.03420526275297622</v>
+        <v>0.07974960814950913</v>
       </c>
     </row>
     <row r="63">
@@ -16008,25 +16008,25 @@
         <v>0.0122008364294054</v>
       </c>
       <c r="BW63" t="n">
-        <v>1339</v>
+        <v>1336.5</v>
       </c>
       <c r="BX63" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY63" s="2" t="n">
         <v>44762.2396180787</v>
       </c>
       <c r="BZ63" t="n">
-        <v>40.088</v>
+        <v>40.08900000000001</v>
       </c>
       <c r="CA63" t="n">
-        <v>0.004472135955001471</v>
+        <v>0.003162277660170497</v>
       </c>
       <c r="CB63" t="n">
-        <v>80.59399999999999</v>
+        <v>80.66599999999998</v>
       </c>
       <c r="CC63" t="n">
-        <v>0.03911521443120847</v>
+        <v>0.08921883209278077</v>
       </c>
     </row>
     <row r="64">
@@ -16253,25 +16253,25 @@
         <v>0.0126334472046245</v>
       </c>
       <c r="BW64" t="n">
-        <v>1358</v>
+        <v>1355.5</v>
       </c>
       <c r="BX64" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY64" s="2" t="n">
         <v>44762.30559030092</v>
       </c>
       <c r="BZ64" t="n">
-        <v>40.09</v>
+        <v>40.08600000000001</v>
       </c>
       <c r="CA64" t="n">
-        <v>0</v>
+        <v>0.008432740427116661</v>
       </c>
       <c r="CB64" t="n">
-        <v>64.792</v>
+        <v>64.876</v>
       </c>
       <c r="CC64" t="n">
-        <v>0.05019960159204975</v>
+        <v>0.1046900186264207</v>
       </c>
     </row>
     <row r="65">
@@ -16498,25 +16498,25 @@
         <v>0.00730693608837637</v>
       </c>
       <c r="BW65" t="n">
-        <v>1376</v>
+        <v>1373.5</v>
       </c>
       <c r="BX65" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY65" s="2" t="n">
         <v>44762.36809030092</v>
       </c>
       <c r="BZ65" t="n">
-        <v>40.09</v>
+        <v>40.08800000000001</v>
       </c>
       <c r="CA65" t="n">
-        <v>0</v>
+        <v>0.006324555320340035</v>
       </c>
       <c r="CB65" t="n">
-        <v>48.78599999999999</v>
+        <v>48.859</v>
       </c>
       <c r="CC65" t="n">
-        <v>0.02880972058177942</v>
+        <v>0.08748968193132546</v>
       </c>
     </row>
     <row r="66">
@@ -16743,25 +16743,25 @@
         <v>0.00401133638645595</v>
       </c>
       <c r="BW66" t="n">
-        <v>1394</v>
+        <v>1391.5</v>
       </c>
       <c r="BX66" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY66" s="2" t="n">
         <v>44762.43059030092</v>
       </c>
       <c r="BZ66" t="n">
-        <v>40.09</v>
+        <v>40.09000000000001</v>
       </c>
       <c r="CA66" t="n">
         <v>0</v>
       </c>
       <c r="CB66" t="n">
-        <v>32.412</v>
+        <v>32.473</v>
       </c>
       <c r="CC66" t="n">
-        <v>0.03346640106136011</v>
+        <v>0.08000694414306249</v>
       </c>
     </row>
     <row r="67">
@@ -16988,25 +16988,25 @@
         <v>0.00100466147601171</v>
       </c>
       <c r="BW67" t="n">
-        <v>1412</v>
+        <v>1409.5</v>
       </c>
       <c r="BX67" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY67" s="2" t="n">
         <v>44762.49309030092</v>
       </c>
       <c r="BZ67" t="n">
-        <v>40.13</v>
+        <v>40.117</v>
       </c>
       <c r="CA67" t="n">
-        <v>0</v>
+        <v>0.01494434118097141</v>
       </c>
       <c r="CB67" t="n">
-        <v>14.562</v>
+        <v>14.621</v>
       </c>
       <c r="CC67" t="n">
-        <v>0.03193743884534253</v>
+        <v>0.08345990387938132</v>
       </c>
     </row>
     <row r="68">
@@ -17233,25 +17233,25 @@
         <v>0.000492324215734649</v>
       </c>
       <c r="BW68" t="n">
-        <v>1449</v>
+        <v>1446.5</v>
       </c>
       <c r="BX68" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY68" s="2" t="n">
         <v>44762.62156252315</v>
       </c>
       <c r="BZ68" t="n">
-        <v>20.306</v>
+        <v>20.464</v>
       </c>
       <c r="CA68" t="n">
-        <v>0.07829431652425466</v>
+        <v>0.1989528140595697</v>
       </c>
       <c r="CB68" t="n">
-        <v>13.612</v>
+        <v>13.545</v>
       </c>
       <c r="CC68" t="n">
-        <v>0.04086563348340515</v>
+        <v>0.08922505876216058</v>
       </c>
     </row>
     <row r="69">
@@ -17478,25 +17478,25 @@
         <v>0.00475645861646699</v>
       </c>
       <c r="BW69" t="n">
-        <v>1467</v>
+        <v>1464.5</v>
       </c>
       <c r="BX69" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY69" s="2" t="n">
         <v>44762.68406252315</v>
       </c>
       <c r="BZ69" t="n">
-        <v>20.184</v>
+        <v>20.194</v>
       </c>
       <c r="CA69" t="n">
-        <v>0.01516575088810338</v>
+        <v>0.01897366596101143</v>
       </c>
       <c r="CB69" t="n">
-        <v>30.826</v>
+        <v>30.75</v>
       </c>
       <c r="CC69" t="n">
-        <v>0.04219004621945723</v>
+        <v>0.1013245610238032</v>
       </c>
     </row>
     <row r="70">
@@ -17723,25 +17723,25 @@
         <v>0.00903425121057712</v>
       </c>
       <c r="BW70" t="n">
-        <v>1485</v>
+        <v>1482.5</v>
       </c>
       <c r="BX70" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY70" s="2" t="n">
         <v>44762.74656252315</v>
       </c>
       <c r="BZ70" t="n">
-        <v>20.178</v>
+        <v>20.181</v>
       </c>
       <c r="CA70" t="n">
-        <v>0.008366600265340524</v>
+        <v>0.008755950357707151</v>
       </c>
       <c r="CB70" t="n">
-        <v>46.69</v>
+        <v>46.588</v>
       </c>
       <c r="CC70" t="n">
-        <v>0.02121320343559692</v>
+        <v>0.1241683445076804</v>
       </c>
     </row>
     <row r="71">
@@ -17968,25 +17968,25 @@
         <v>0.0189592297642696</v>
       </c>
       <c r="BW71" t="n">
-        <v>1504</v>
+        <v>1501.5</v>
       </c>
       <c r="BX71" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY71" s="2" t="n">
         <v>44762.81253474537</v>
       </c>
       <c r="BZ71" t="n">
-        <v>20.192</v>
+        <v>20.196</v>
       </c>
       <c r="CA71" t="n">
-        <v>0.008366600265340099</v>
+        <v>0.009660917830792252</v>
       </c>
       <c r="CB71" t="n">
-        <v>62.51799999999999</v>
+        <v>62.40600000000001</v>
       </c>
       <c r="CC71" t="n">
-        <v>0.05310367218940776</v>
+        <v>0.1392998364839136</v>
       </c>
     </row>
     <row r="72">
@@ -18213,25 +18213,25 @@
         <v>0.0155031977365252</v>
       </c>
       <c r="BW72" t="n">
-        <v>1522</v>
+        <v>1519.5</v>
       </c>
       <c r="BX72" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY72" s="2" t="n">
         <v>44762.87503474537</v>
       </c>
       <c r="BZ72" t="n">
-        <v>20.198</v>
+        <v>20.20499999999999</v>
       </c>
       <c r="CA72" t="n">
-        <v>0.004472135954999402</v>
+        <v>0.009718253158074426</v>
       </c>
       <c r="CB72" t="n">
-        <v>78.374</v>
+        <v>78.22199999999999</v>
       </c>
       <c r="CC72" t="n">
-        <v>0.0918150314491063</v>
+        <v>0.1864164990313721</v>
       </c>
     </row>
     <row r="73">
@@ -18458,25 +18458,25 @@
         <v>0.0049638874654986</v>
       </c>
       <c r="BW73" t="n">
-        <v>1558</v>
+        <v>1555.5</v>
       </c>
       <c r="BX73" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY73" s="2" t="n">
         <v>44763.00003474537</v>
       </c>
       <c r="BZ73" t="n">
-        <v>20.194</v>
+        <v>20.197</v>
       </c>
       <c r="CA73" t="n">
-        <v>0.008944271909998604</v>
+        <v>0.006749485577104801</v>
       </c>
       <c r="CB73" t="n">
-        <v>95.39399999999999</v>
+        <v>95.29300000000001</v>
       </c>
       <c r="CC73" t="n">
-        <v>0.05224940191045517</v>
+        <v>0.1219334973572826</v>
       </c>
     </row>
     <row r="74">
@@ -18703,25 +18703,25 @@
         <v>0.0174102914835116</v>
       </c>
       <c r="BW74" t="n">
-        <v>1576</v>
+        <v>1573.5</v>
       </c>
       <c r="BX74" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY74" s="2" t="n">
         <v>44763.06253474537</v>
       </c>
       <c r="BZ74" t="n">
-        <v>20.128</v>
+        <v>20.124</v>
       </c>
       <c r="CA74" t="n">
-        <v>0.019235384061671</v>
+        <v>0.01429840705968443</v>
       </c>
       <c r="CB74" t="n">
-        <v>80.88800000000001</v>
+        <v>81</v>
       </c>
       <c r="CC74" t="n">
-        <v>0.05718391382198715</v>
+        <v>0.1358921140709265</v>
       </c>
     </row>
     <row r="75">
@@ -18948,25 +18948,25 @@
         <v>0.0161950687766729</v>
       </c>
       <c r="BW75" t="n">
-        <v>1594</v>
+        <v>1591.5</v>
       </c>
       <c r="BX75" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY75" s="2" t="n">
         <v>44763.12503474537</v>
       </c>
       <c r="BZ75" t="n">
-        <v>20.136</v>
+        <v>20.12499999999999</v>
       </c>
       <c r="CA75" t="n">
-        <v>0.005477225575053031</v>
+        <v>0.01354006400772585</v>
       </c>
       <c r="CB75" t="n">
-        <v>65.098</v>
+        <v>65.215</v>
       </c>
       <c r="CC75" t="n">
-        <v>0.05215361924162037</v>
+        <v>0.1425365450214967</v>
       </c>
     </row>
     <row r="76">
@@ -19193,25 +19193,25 @@
         <v>0.00714137340095897</v>
       </c>
       <c r="BW76" t="n">
-        <v>1612</v>
+        <v>1609.5</v>
       </c>
       <c r="BX76" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY76" s="2" t="n">
         <v>44763.18753474537</v>
       </c>
       <c r="BZ76" t="n">
-        <v>20.108</v>
+        <v>20.104</v>
       </c>
       <c r="CA76" t="n">
-        <v>0.008366600265340364</v>
+        <v>0.008432740427114623</v>
       </c>
       <c r="CB76" t="n">
-        <v>48.922</v>
+        <v>49.02800000000001</v>
       </c>
       <c r="CC76" t="n">
-        <v>0.04604345773288489</v>
+        <v>0.1301964327895002</v>
       </c>
     </row>
     <row r="77">
@@ -19438,25 +19438,25 @@
         <v>0.00514794685606825</v>
       </c>
       <c r="BW77" t="n">
-        <v>1630</v>
+        <v>1627.5</v>
       </c>
       <c r="BX77" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY77" s="2" t="n">
         <v>44763.25003474537</v>
       </c>
       <c r="BZ77" t="n">
-        <v>20.098</v>
+        <v>20.095</v>
       </c>
       <c r="CA77" t="n">
-        <v>0.00836660026534178</v>
+        <v>0.008498365855988382</v>
       </c>
       <c r="CB77" t="n">
-        <v>32.604</v>
+        <v>32.70800000000001</v>
       </c>
       <c r="CC77" t="n">
-        <v>0.04878524367060028</v>
+        <v>0.1279583265494428</v>
       </c>
     </row>
     <row r="78">
@@ -19683,25 +19683,25 @@
         <v>0.000582871752086893</v>
       </c>
       <c r="BW78" t="n">
-        <v>1649</v>
+        <v>1646.5</v>
       </c>
       <c r="BX78" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY78" s="2" t="n">
         <v>44763.31600696759</v>
       </c>
       <c r="BZ78" t="n">
-        <v>20.088</v>
+        <v>20.089</v>
       </c>
       <c r="CA78" t="n">
-        <v>0.01095445115010488</v>
+        <v>0.008755950357709059</v>
       </c>
       <c r="CB78" t="n">
-        <v>14.57</v>
+        <v>14.648</v>
       </c>
       <c r="CC78" t="n">
-        <v>0.04898979485566279</v>
+        <v>0.09852241707685938</v>
       </c>
     </row>
     <row r="79">
@@ -19928,10 +19928,10 @@
         <v>0.000691880543981738</v>
       </c>
       <c r="BW79" t="n">
-        <v>1685</v>
+        <v>1682.5</v>
       </c>
       <c r="BX79" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY79" s="2" t="n">
         <v>44763.44100696759</v>
@@ -19940,13 +19940,13 @@
         <v>20.13</v>
       </c>
       <c r="CA79" t="n">
-        <v>0.007071067811864958</v>
+        <v>0.006666666666667</v>
       </c>
       <c r="CB79" t="n">
-        <v>14.118</v>
+        <v>14.128</v>
       </c>
       <c r="CC79" t="n">
-        <v>0.01643167672515561</v>
+        <v>0.01932183566158569</v>
       </c>
     </row>
     <row r="80">
@@ -20173,25 +20173,25 @@
         <v>0.00780467478148381</v>
       </c>
       <c r="BW80" t="n">
-        <v>1703</v>
+        <v>1700.5</v>
       </c>
       <c r="BX80" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY80" s="2" t="n">
         <v>44763.50350696759</v>
       </c>
       <c r="BZ80" t="n">
-        <v>20.138</v>
+        <v>20.13699999999999</v>
       </c>
       <c r="CA80" t="n">
-        <v>0.004472135955000676</v>
+        <v>0.01059349905471449</v>
       </c>
       <c r="CB80" t="n">
-        <v>31.352</v>
+        <v>31.308</v>
       </c>
       <c r="CC80" t="n">
-        <v>0.02489979919597781</v>
+        <v>0.05788878225624721</v>
       </c>
     </row>
     <row r="81">
@@ -20418,25 +20418,25 @@
         <v>0.0258870017077982</v>
       </c>
       <c r="BW81" t="n">
-        <v>1734</v>
+        <v>1731.5</v>
       </c>
       <c r="BX81" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY81" s="2" t="n">
         <v>44763.61114585648</v>
       </c>
       <c r="BZ81" t="n">
-        <v>20.146</v>
+        <v>20.15</v>
       </c>
       <c r="CA81" t="n">
-        <v>0.01949358868961695</v>
+        <v>0.01632993161855448</v>
       </c>
       <c r="CB81" t="n">
-        <v>47.43599999999999</v>
+        <v>47.41999999999999</v>
       </c>
       <c r="CC81" t="n">
-        <v>0.02880972058177741</v>
+        <v>0.0270801280154539</v>
       </c>
     </row>
     <row r="82">
@@ -20663,10 +20663,10 @@
         <v>0.0316631299426245</v>
       </c>
       <c r="BW82" t="n">
-        <v>1752</v>
+        <v>1749.5</v>
       </c>
       <c r="BX82" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY82" s="2" t="n">
         <v>44763.67364585648</v>
@@ -20675,13 +20675,13 @@
         <v>20.186</v>
       </c>
       <c r="CA82" t="n">
-        <v>0.01140175425099096</v>
+        <v>0.009660917830792435</v>
       </c>
       <c r="CB82" t="n">
-        <v>62.916</v>
+        <v>62.83300000000001</v>
       </c>
       <c r="CC82" t="n">
-        <v>0.03130495168499937</v>
+        <v>0.1017677093515795</v>
       </c>
     </row>
     <row r="83">
@@ -20908,10 +20908,10 @@
         <v>0.032408821672357</v>
       </c>
       <c r="BW83" t="n">
-        <v>1771</v>
+        <v>1768.5</v>
       </c>
       <c r="BX83" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY83" s="2" t="n">
         <v>44763.7396180787</v>
@@ -20920,13 +20920,13 @@
         <v>20.198</v>
       </c>
       <c r="CA83" t="n">
-        <v>0.01095445115010393</v>
+        <v>0.007888106377466257</v>
       </c>
       <c r="CB83" t="n">
-        <v>78.616</v>
+        <v>78.479</v>
       </c>
       <c r="CC83" t="n">
-        <v>0.06730527468185385</v>
+        <v>0.1656267557558923</v>
       </c>
     </row>
     <row r="84">
@@ -21153,25 +21153,25 @@
         <v>0.00753927281274647</v>
       </c>
       <c r="BW84" t="n">
-        <v>1795</v>
+        <v>1792.5</v>
       </c>
       <c r="BX84" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY84" s="2" t="n">
         <v>44763.82295141204</v>
       </c>
       <c r="BZ84" t="n">
-        <v>20.224</v>
+        <v>20.226</v>
       </c>
       <c r="CA84" t="n">
-        <v>0.005477225575053031</v>
+        <v>0.005163977794943854</v>
       </c>
       <c r="CB84" t="n">
-        <v>94.818</v>
+        <v>94.65899999999999</v>
       </c>
       <c r="CC84" t="n">
-        <v>0.08927485648265694</v>
+        <v>0.193474086694377</v>
       </c>
     </row>
     <row r="85">
@@ -21398,25 +21398,25 @@
         <v>0.0398908272762644</v>
       </c>
       <c r="BW85" t="n">
-        <v>1813</v>
+        <v>1810.5</v>
       </c>
       <c r="BX85" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY85" s="2" t="n">
         <v>44763.88545141204</v>
       </c>
       <c r="BZ85" t="n">
-        <v>20.136</v>
+        <v>20.129</v>
       </c>
       <c r="CA85" t="n">
-        <v>0.00547722557505249</v>
+        <v>0.008755950357706764</v>
       </c>
       <c r="CB85" t="n">
-        <v>80.52200000000001</v>
+        <v>80.61199999999999</v>
       </c>
       <c r="CC85" t="n">
-        <v>0.03420526275298006</v>
+        <v>0.1110355298491811</v>
       </c>
     </row>
     <row r="86">
@@ -21643,25 +21643,25 @@
         <v>0.0275993843498875</v>
       </c>
       <c r="BW86" t="n">
-        <v>1831</v>
+        <v>1828.5</v>
       </c>
       <c r="BX86" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY86" s="2" t="n">
         <v>44763.94795141204</v>
       </c>
       <c r="BZ86" t="n">
-        <v>20.13</v>
+        <v>20.125</v>
       </c>
       <c r="CA86" t="n">
-        <v>0.007071067811864382</v>
+        <v>0.01178511301977528</v>
       </c>
       <c r="CB86" t="n">
-        <v>64.956</v>
+        <v>65.068</v>
       </c>
       <c r="CC86" t="n">
-        <v>0.0618869937870627</v>
+        <v>0.1369346965203123</v>
       </c>
     </row>
     <row r="87">
@@ -21888,25 +21888,25 @@
         <v>0.020485891640412</v>
       </c>
       <c r="BW87" t="n">
-        <v>1849</v>
+        <v>1846.5</v>
       </c>
       <c r="BX87" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY87" s="2" t="n">
         <v>44764.01045141204</v>
       </c>
       <c r="BZ87" t="n">
-        <v>20.098</v>
+        <v>20.096</v>
       </c>
       <c r="CA87" t="n">
-        <v>0.010954451150104</v>
+        <v>0.01074967699773171</v>
       </c>
       <c r="CB87" t="n">
-        <v>48.896</v>
+        <v>48.986</v>
       </c>
       <c r="CC87" t="n">
-        <v>0.06426507605223697</v>
+        <v>0.1141344236708051</v>
       </c>
     </row>
     <row r="88">
@@ -22133,25 +22133,25 @@
         <v>0.0052275755278891</v>
       </c>
       <c r="BW88" t="n">
-        <v>1867</v>
+        <v>1864.5</v>
       </c>
       <c r="BX88" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY88" s="2" t="n">
         <v>44764.07295141204</v>
       </c>
       <c r="BZ88" t="n">
-        <v>20.092</v>
+        <v>20.09</v>
       </c>
       <c r="CA88" t="n">
-        <v>0.008366600265341922</v>
+        <v>0.01054092553389537</v>
       </c>
       <c r="CB88" t="n">
-        <v>32.604</v>
+        <v>32.69600000000001</v>
       </c>
       <c r="CC88" t="n">
-        <v>0.04878524367060028</v>
+        <v>0.1153930481249038</v>
       </c>
     </row>
     <row r="89">
@@ -22378,25 +22378,25 @@
         <v>0.000828404009296152</v>
       </c>
       <c r="BW89" t="n">
-        <v>1885</v>
+        <v>1882.5</v>
       </c>
       <c r="BX89" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY89" s="2" t="n">
         <v>44764.13545141204</v>
       </c>
       <c r="BZ89" t="n">
-        <v>20.094</v>
+        <v>20.088</v>
       </c>
       <c r="CA89" t="n">
-        <v>0.005477225575052301</v>
+        <v>0.01032795558988603</v>
       </c>
       <c r="CB89" t="n">
-        <v>14.594</v>
+        <v>14.679</v>
       </c>
       <c r="CC89" t="n">
-        <v>0.05366563145999472</v>
+        <v>0.1057722921079889</v>
       </c>
     </row>
     <row r="90">
@@ -22623,19 +22623,19 @@
         <v>0.0028333772955469</v>
       </c>
       <c r="BW90" t="n">
-        <v>1957</v>
+        <v>1954.5</v>
       </c>
       <c r="BX90" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY90" s="2" t="n">
         <v>44764.38545141204</v>
       </c>
       <c r="BZ90" t="n">
-        <v>0.208</v>
+        <v>0.213</v>
       </c>
       <c r="CA90" t="n">
-        <v>0.01643167672515498</v>
+        <v>0.01251665557034573</v>
       </c>
       <c r="CB90" t="n">
         <v>13.77</v>
@@ -22868,25 +22868,25 @@
         <v>0.0148347686073546</v>
       </c>
       <c r="BW91" t="n">
-        <v>1975</v>
+        <v>1972.5</v>
       </c>
       <c r="BX91" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY91" s="2" t="n">
         <v>44764.44795141204</v>
       </c>
       <c r="BZ91" t="n">
-        <v>0.216</v>
+        <v>0.213</v>
       </c>
       <c r="CA91" t="n">
-        <v>0.005477225575051664</v>
+        <v>0.004830458915396477</v>
       </c>
       <c r="CB91" t="n">
-        <v>30.80399999999999</v>
+        <v>30.70500000000001</v>
       </c>
       <c r="CC91" t="n">
-        <v>0.04878524367060216</v>
+        <v>0.1215867317322654</v>
       </c>
     </row>
     <row r="92">
@@ -23113,25 +23113,25 @@
         <v>0.0255815443061462</v>
       </c>
       <c r="BW92" t="n">
-        <v>1994</v>
+        <v>1991.5</v>
       </c>
       <c r="BX92" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY92" s="2" t="n">
         <v>44764.51392363426</v>
       </c>
       <c r="BZ92" t="n">
-        <v>0.23</v>
+        <v>0.232</v>
       </c>
       <c r="CA92" t="n">
-        <v>0</v>
+        <v>0.006324555320336755</v>
       </c>
       <c r="CB92" t="n">
-        <v>46.70999999999999</v>
+        <v>46.583</v>
       </c>
       <c r="CC92" t="n">
-        <v>0.06519202405202246</v>
+        <v>0.1519539403898433</v>
       </c>
     </row>
     <row r="93">
@@ -23358,25 +23358,25 @@
         <v>0.039476763915676</v>
       </c>
       <c r="BW93" t="n">
-        <v>2012</v>
+        <v>2009.5</v>
       </c>
       <c r="BX93" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY93" s="2" t="n">
         <v>44764.57642363426</v>
       </c>
       <c r="BZ93" t="n">
-        <v>0.23</v>
+        <v>0.233</v>
       </c>
       <c r="CA93" t="n">
-        <v>0</v>
+        <v>0.009486832980505124</v>
       </c>
       <c r="CB93" t="n">
-        <v>62.58</v>
+        <v>62.42100000000001</v>
       </c>
       <c r="CC93" t="n">
-        <v>0.06670832032063018</v>
+        <v>0.1882344873348734</v>
       </c>
     </row>
     <row r="94">
@@ -23603,25 +23603,25 @@
         <v>0.0326753170470097</v>
       </c>
       <c r="BW94" t="n">
-        <v>2031</v>
+        <v>2028.5</v>
       </c>
       <c r="BX94" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY94" s="2" t="n">
         <v>44764.64239585648</v>
       </c>
       <c r="BZ94" t="n">
-        <v>0.266</v>
+        <v>0.265</v>
       </c>
       <c r="CA94" t="n">
-        <v>0.005477225575051667</v>
+        <v>0.005270462766947306</v>
       </c>
       <c r="CB94" t="n">
-        <v>78.458</v>
+        <v>78.26700000000001</v>
       </c>
       <c r="CC94" t="n">
-        <v>0.09984988733092548</v>
+        <v>0.2328113208396749</v>
       </c>
     </row>
     <row r="95">
@@ -23848,25 +23848,25 @@
         <v>0.008235432385299829</v>
       </c>
       <c r="BW95" t="n">
-        <v>2067</v>
+        <v>2064.5</v>
       </c>
       <c r="BX95" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY95" s="2" t="n">
         <v>44764.76739585648</v>
       </c>
       <c r="BZ95" t="n">
-        <v>0.268</v>
+        <v>0.267</v>
       </c>
       <c r="CA95" t="n">
-        <v>0.00447213595499958</v>
+        <v>0.004830458915396483</v>
       </c>
       <c r="CB95" t="n">
-        <v>95.31400000000001</v>
+        <v>95.19299999999998</v>
       </c>
       <c r="CC95" t="n">
-        <v>0.07797435475847365</v>
+        <v>0.1507057471439702</v>
       </c>
     </row>
     <row r="96">
@@ -24093,25 +24093,25 @@
         <v>0.0264277636112268</v>
       </c>
       <c r="BW96" t="n">
-        <v>2085</v>
+        <v>2082.5</v>
       </c>
       <c r="BX96" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY96" s="2" t="n">
         <v>44764.82989585648</v>
       </c>
       <c r="BZ96" t="n">
-        <v>0.22</v>
+        <v>0.216</v>
       </c>
       <c r="CA96" t="n">
-        <v>0.007071067811865481</v>
+        <v>0.006992058987801007</v>
       </c>
       <c r="CB96" t="n">
-        <v>81.47</v>
+        <v>81.59300000000002</v>
       </c>
       <c r="CC96" t="n">
-        <v>0.05431390245600112</v>
+        <v>0.1508531294559955</v>
       </c>
     </row>
     <row r="97">
@@ -24338,25 +24338,25 @@
         <v>0.0326046662181376</v>
       </c>
       <c r="BW97" t="n">
-        <v>2103</v>
+        <v>2100.5</v>
       </c>
       <c r="BX97" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY97" s="2" t="n">
         <v>44764.89239585648</v>
       </c>
       <c r="BZ97" t="n">
-        <v>0.214</v>
+        <v>0.212</v>
       </c>
       <c r="CA97" t="n">
-        <v>0.005477225575051667</v>
+        <v>0.004216370213557843</v>
       </c>
       <c r="CB97" t="n">
-        <v>65.866</v>
+        <v>66.03299999999999</v>
       </c>
       <c r="CC97" t="n">
-        <v>0.07436396977031771</v>
+        <v>0.2101348773208875</v>
       </c>
     </row>
     <row r="98">
@@ -24583,25 +24583,25 @@
         <v>0.0227526270537121</v>
       </c>
       <c r="BW98" t="n">
-        <v>2121</v>
+        <v>2118.5</v>
       </c>
       <c r="BX98" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY98" s="2" t="n">
         <v>44764.95489585648</v>
       </c>
       <c r="BZ98" t="n">
-        <v>0.214</v>
+        <v>0.212</v>
       </c>
       <c r="CA98" t="n">
-        <v>0.005477225575051669</v>
+        <v>0.004216370213557842</v>
       </c>
       <c r="CB98" t="n">
-        <v>49.532</v>
+        <v>49.685</v>
       </c>
       <c r="CC98" t="n">
-        <v>0.0769415362466872</v>
+        <v>0.1861451046898637</v>
       </c>
     </row>
     <row r="99">
@@ -24828,25 +24828,25 @@
         <v>0.011301641087936</v>
       </c>
       <c r="BW99" t="n">
-        <v>2140</v>
+        <v>2137.5</v>
       </c>
       <c r="BX99" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY99" s="2" t="n">
         <v>44765.0208680787</v>
       </c>
       <c r="BZ99" t="n">
-        <v>0.186</v>
+        <v>0.183</v>
       </c>
       <c r="CA99" t="n">
-        <v>0.01341640786499874</v>
+        <v>0.009486832980505139</v>
       </c>
       <c r="CB99" t="n">
-        <v>33.024</v>
+        <v>33.156</v>
       </c>
       <c r="CC99" t="n">
-        <v>0.06542170893518455</v>
+        <v>0.1618092155046298</v>
       </c>
     </row>
     <row r="100">
@@ -25073,10 +25073,10 @@
         <v>0.00218600737320124</v>
       </c>
       <c r="BW100" t="n">
-        <v>2158</v>
+        <v>2155.5</v>
       </c>
       <c r="BX100" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY100" s="2" t="n">
         <v>44765.0833680787</v>
@@ -25088,10 +25088,10 @@
         <v>0</v>
       </c>
       <c r="CB100" t="n">
-        <v>15.102</v>
+        <v>15.252</v>
       </c>
       <c r="CC100" t="n">
-        <v>0.09523654760647264</v>
+        <v>0.1854603881036479</v>
       </c>
     </row>
     <row r="101">
@@ -25318,25 +25318,25 @@
         <v>0.00114595751304314</v>
       </c>
       <c r="BW101" t="n">
-        <v>2194</v>
+        <v>2191.5</v>
       </c>
       <c r="BX101" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY101" s="2" t="n">
         <v>44765.2083680787</v>
       </c>
       <c r="BZ101" t="n">
-        <v>10.006</v>
+        <v>9.936</v>
       </c>
       <c r="CA101" t="n">
-        <v>0.03049590136395242</v>
+        <v>0.08553102101317112</v>
       </c>
       <c r="CB101" t="n">
-        <v>14.516</v>
+        <v>14.592</v>
       </c>
       <c r="CC101" t="n">
-        <v>0.04878524367060168</v>
+        <v>0.101631141334183</v>
       </c>
     </row>
     <row r="102">
@@ -25563,25 +25563,25 @@
         <v>0.0155654348092924</v>
       </c>
       <c r="BW102" t="n">
-        <v>2212</v>
+        <v>2209.5</v>
       </c>
       <c r="BX102" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY102" s="2" t="n">
         <v>44765.2708680787</v>
       </c>
       <c r="BZ102" t="n">
-        <v>10.106</v>
+        <v>10.102</v>
       </c>
       <c r="CA102" t="n">
-        <v>0.008944271909998911</v>
+        <v>0.00918936583472685</v>
       </c>
       <c r="CB102" t="n">
-        <v>31.69400000000001</v>
+        <v>31.65</v>
       </c>
       <c r="CC102" t="n">
-        <v>0.02190890230020642</v>
+        <v>0.05849976258261431</v>
       </c>
     </row>
     <row r="103">
@@ -25808,25 +25808,25 @@
         <v>0.020471116606051</v>
       </c>
       <c r="BW103" t="n">
-        <v>2230</v>
+        <v>2227.5</v>
       </c>
       <c r="BX103" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY103" s="2" t="n">
         <v>44765.3333680787</v>
       </c>
       <c r="BZ103" t="n">
-        <v>10.138</v>
+        <v>10.137</v>
       </c>
       <c r="CA103" t="n">
-        <v>0.004472135954998764</v>
+        <v>0.004830458915395982</v>
       </c>
       <c r="CB103" t="n">
-        <v>47.48200000000001</v>
+        <v>47.37399999999999</v>
       </c>
       <c r="CC103" t="n">
-        <v>0.03633180424916944</v>
+        <v>0.1227644537767787</v>
       </c>
     </row>
     <row r="104">
@@ -26053,25 +26053,25 @@
         <v>0.0353885087403893</v>
       </c>
       <c r="BW104" t="n">
-        <v>2248</v>
+        <v>2245.5</v>
       </c>
       <c r="BX104" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY104" s="2" t="n">
         <v>44765.3958680787</v>
       </c>
       <c r="BZ104" t="n">
-        <v>10.13</v>
+        <v>10.145</v>
       </c>
       <c r="CA104" t="n">
-        <v>0</v>
+        <v>0.01840893502864573</v>
       </c>
       <c r="CB104" t="n">
-        <v>63.194</v>
+        <v>63.075</v>
       </c>
       <c r="CC104" t="n">
-        <v>0.06655824516917663</v>
+        <v>0.1467613330850113</v>
       </c>
     </row>
     <row r="105">
@@ -26298,10 +26298,10 @@
         <v>0.0269755401171174</v>
       </c>
       <c r="BW105" t="n">
-        <v>2267</v>
+        <v>2264.5</v>
       </c>
       <c r="BX105" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY105" s="2" t="n">
         <v>44765.46184030092</v>
@@ -26310,13 +26310,13 @@
         <v>10.172</v>
       </c>
       <c r="CA105" t="n">
-        <v>0.004472135954999509</v>
+        <v>0.004216370213557738</v>
       </c>
       <c r="CB105" t="n">
-        <v>78.908</v>
+        <v>78.755</v>
       </c>
       <c r="CC105" t="n">
-        <v>0.06978538528948172</v>
+        <v>0.1821629307332756</v>
       </c>
     </row>
     <row r="106">
@@ -26543,25 +26543,25 @@
         <v>0.0141532959097415</v>
       </c>
       <c r="BW106" t="n">
-        <v>2303</v>
+        <v>2300.5</v>
       </c>
       <c r="BX106" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY106" s="2" t="n">
         <v>44765.58684030092</v>
       </c>
       <c r="BZ106" t="n">
-        <v>10.172</v>
+        <v>10.176</v>
       </c>
       <c r="CA106" t="n">
-        <v>0.004472135954999302</v>
+        <v>0.008432740427115219</v>
       </c>
       <c r="CB106" t="n">
-        <v>95.60599999999999</v>
+        <v>95.52</v>
       </c>
       <c r="CC106" t="n">
-        <v>0.06841052550594656</v>
+        <v>0.1085254706406648</v>
       </c>
     </row>
     <row r="107">
@@ -26788,25 +26788,25 @@
         <v>0.0188454313161726</v>
       </c>
       <c r="BW107" t="n">
-        <v>2321</v>
+        <v>2318.5</v>
       </c>
       <c r="BX107" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY107" s="2" t="n">
         <v>44765.64934030092</v>
       </c>
       <c r="BZ107" t="n">
-        <v>10.11</v>
+        <v>10.105</v>
       </c>
       <c r="CA107" t="n">
-        <v>0.007071067811865324</v>
+        <v>0.008498365855987568</v>
       </c>
       <c r="CB107" t="n">
-        <v>81.34400000000001</v>
+        <v>81.465</v>
       </c>
       <c r="CC107" t="n">
-        <v>0.05941380311005046</v>
+        <v>0.1482677757752348</v>
       </c>
     </row>
     <row r="108">
@@ -27033,25 +27033,25 @@
         <v>0.0319523526412133</v>
       </c>
       <c r="BW108" t="n">
-        <v>2340</v>
+        <v>2337.5</v>
       </c>
       <c r="BX108" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY108" s="2" t="n">
         <v>44765.71531252315</v>
       </c>
       <c r="BZ108" t="n">
-        <v>10.096</v>
+        <v>10.092</v>
       </c>
       <c r="CA108" t="n">
-        <v>0.005477225575051653</v>
+        <v>0.007888106377465709</v>
       </c>
       <c r="CB108" t="n">
-        <v>65.562</v>
+        <v>65.69699999999999</v>
       </c>
       <c r="CC108" t="n">
-        <v>0.0697853852894777</v>
+        <v>0.1688556253792721</v>
       </c>
     </row>
     <row r="109">
@@ -27278,25 +27278,25 @@
         <v>0.0228793357390251</v>
       </c>
       <c r="BW109" t="n">
-        <v>2358</v>
+        <v>2355.5</v>
       </c>
       <c r="BX109" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY109" s="2" t="n">
         <v>44765.77781252315</v>
       </c>
       <c r="BZ109" t="n">
-        <v>10.084</v>
+        <v>10.085</v>
       </c>
       <c r="CA109" t="n">
-        <v>0.008944271909999068</v>
+        <v>0.007071067811865074</v>
       </c>
       <c r="CB109" t="n">
-        <v>49.358</v>
+        <v>49.468</v>
       </c>
       <c r="CC109" t="n">
-        <v>0.03420526275297438</v>
+        <v>0.137501515143167</v>
       </c>
     </row>
     <row r="110">
@@ -27523,25 +27523,25 @@
         <v>0.0102687919527308</v>
       </c>
       <c r="BW110" t="n">
-        <v>2376</v>
+        <v>2373.5</v>
       </c>
       <c r="BX110" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY110" s="2" t="n">
         <v>44765.84031252315</v>
       </c>
       <c r="BZ110" t="n">
-        <v>10.082</v>
+        <v>10.078</v>
       </c>
       <c r="CA110" t="n">
-        <v>0.004472135954999219</v>
+        <v>0.01316561177208768</v>
       </c>
       <c r="CB110" t="n">
-        <v>32.984</v>
+        <v>33.07100000000001</v>
       </c>
       <c r="CC110" t="n">
-        <v>0.04449719092257332</v>
+        <v>0.1185514421862686</v>
       </c>
     </row>
     <row r="111">
@@ -27768,25 +27768,25 @@
         <v>0.000857151360388744</v>
       </c>
       <c r="BW111" t="n">
-        <v>2395</v>
+        <v>2392.5</v>
       </c>
       <c r="BX111" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY111" s="2" t="n">
         <v>44765.90628474537</v>
       </c>
       <c r="BZ111" t="n">
-        <v>10.076</v>
+        <v>10.074</v>
       </c>
       <c r="CA111" t="n">
-        <v>0.008944271909998688</v>
+        <v>0.008432740427115039</v>
       </c>
       <c r="CB111" t="n">
-        <v>14.826</v>
+        <v>14.95</v>
       </c>
       <c r="CC111" t="n">
-        <v>0.04560701700396662</v>
+        <v>0.1569854911908897</v>
       </c>
     </row>
     <row r="112">
@@ -28013,25 +28013,25 @@
         <v>0.000434743160915658</v>
       </c>
       <c r="BW112" t="n">
-        <v>2431</v>
+        <v>2428.5</v>
       </c>
       <c r="BX112" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY112" s="2" t="n">
         <v>44766.03128474537</v>
       </c>
       <c r="BZ112" t="n">
-        <v>19.958</v>
+        <v>19.896</v>
       </c>
       <c r="CA112" t="n">
-        <v>0.05118593556827974</v>
+        <v>0.08235424835563844</v>
       </c>
       <c r="CB112" t="n">
-        <v>14.364</v>
+        <v>14.448</v>
       </c>
       <c r="CC112" t="n">
-        <v>0.03507135583350078</v>
+        <v>0.1005319186461032</v>
       </c>
     </row>
     <row r="113">
@@ -28258,25 +28258,25 @@
         <v>0.00980346533770193</v>
       </c>
       <c r="BW113" t="n">
-        <v>2449</v>
+        <v>2446.5</v>
       </c>
       <c r="BX113" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY113" s="2" t="n">
         <v>44766.09378474537</v>
       </c>
       <c r="BZ113" t="n">
-        <v>20.118</v>
+        <v>20.117</v>
       </c>
       <c r="CA113" t="n">
-        <v>0.00836660026534017</v>
+        <v>0.008232726023485558</v>
       </c>
       <c r="CB113" t="n">
-        <v>31.574</v>
+        <v>31.544</v>
       </c>
       <c r="CC113" t="n">
-        <v>0.02190890230020642</v>
+        <v>0.04195235392680394</v>
       </c>
     </row>
     <row r="114">
@@ -28503,25 +28503,25 @@
         <v>0.0155632717985066</v>
       </c>
       <c r="BW114" t="n">
-        <v>2468</v>
+        <v>2465.5</v>
       </c>
       <c r="BX114" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY114" s="2" t="n">
         <v>44766.15975696759</v>
       </c>
       <c r="BZ114" t="n">
-        <v>20.142</v>
+        <v>20.149</v>
       </c>
       <c r="CA114" t="n">
-        <v>0.01095445115010353</v>
+        <v>0.01197218999737952</v>
       </c>
       <c r="CB114" t="n">
-        <v>47.364</v>
+        <v>47.309</v>
       </c>
       <c r="CC114" t="n">
-        <v>0.03911521443121675</v>
+        <v>0.07264066813202148</v>
       </c>
     </row>
     <row r="115">
@@ -28748,25 +28748,25 @@
         <v>0.0280062390371878</v>
       </c>
       <c r="BW115" t="n">
-        <v>2486</v>
+        <v>2483.5</v>
       </c>
       <c r="BX115" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY115" s="2" t="n">
         <v>44766.22225696759</v>
       </c>
       <c r="BZ115" t="n">
-        <v>20.174</v>
+        <v>20.179</v>
       </c>
       <c r="CA115" t="n">
-        <v>0.01140175425099267</v>
+        <v>0.01197218999737822</v>
       </c>
       <c r="CB115" t="n">
-        <v>63.062</v>
+        <v>62.972</v>
       </c>
       <c r="CC115" t="n">
-        <v>0.05019960159204247</v>
+        <v>0.1098281485877871</v>
       </c>
     </row>
     <row r="116">
@@ -28993,25 +28993,25 @@
         <v>0.0227458372619047</v>
       </c>
       <c r="BW116" t="n">
-        <v>2505</v>
+        <v>2502.5</v>
       </c>
       <c r="BX116" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY116" s="2" t="n">
         <v>44766.28822918981</v>
       </c>
       <c r="BZ116" t="n">
-        <v>20.198</v>
+        <v>20.197</v>
       </c>
       <c r="CA116" t="n">
-        <v>0.004472135954999402</v>
+        <v>0.006749485577105283</v>
       </c>
       <c r="CB116" t="n">
-        <v>78.72999999999999</v>
+        <v>78.60899999999999</v>
       </c>
       <c r="CC116" t="n">
-        <v>0.05431390245600832</v>
+        <v>0.1483576759052266</v>
       </c>
     </row>
     <row r="117">
@@ -29238,25 +29238,25 @@
         <v>0.00856331530715855</v>
       </c>
       <c r="BW117" t="n">
-        <v>2541</v>
+        <v>2538.5</v>
       </c>
       <c r="BX117" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY117" s="2" t="n">
         <v>44766.41322918981</v>
       </c>
       <c r="BZ117" t="n">
-        <v>20.188</v>
+        <v>20.195</v>
       </c>
       <c r="CA117" t="n">
-        <v>0.01643167672515443</v>
+        <v>0.01354006400772687</v>
       </c>
       <c r="CB117" t="n">
-        <v>95.374</v>
+        <v>95.283</v>
       </c>
       <c r="CC117" t="n">
-        <v>0.06188699378705676</v>
+        <v>0.1123536084571079</v>
       </c>
     </row>
     <row r="118">
@@ -29483,10 +29483,10 @@
         <v>0.0239228812372073</v>
       </c>
       <c r="BW118" t="n">
-        <v>2559</v>
+        <v>2556.5</v>
       </c>
       <c r="BX118" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY118" s="2" t="n">
         <v>44766.47572918981</v>
@@ -29495,13 +29495,13 @@
         <v>20.126</v>
       </c>
       <c r="CA118" t="n">
-        <v>0.005477225575050004</v>
+        <v>0.00966091783079207</v>
       </c>
       <c r="CB118" t="n">
-        <v>80.926</v>
+        <v>81.03299999999999</v>
       </c>
       <c r="CC118" t="n">
-        <v>0.0634822809924146</v>
+        <v>0.1359779393872454</v>
       </c>
     </row>
     <row r="119">
@@ -29728,25 +29728,25 @@
         <v>0.0257524309321192</v>
       </c>
       <c r="BW119" t="n">
-        <v>2577</v>
+        <v>2574.5</v>
       </c>
       <c r="BX119" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY119" s="2" t="n">
         <v>44766.53822918981</v>
       </c>
       <c r="BZ119" t="n">
-        <v>20.128</v>
+        <v>20.119</v>
       </c>
       <c r="CA119" t="n">
-        <v>0.01095445115010387</v>
+        <v>0.0137032031940617</v>
       </c>
       <c r="CB119" t="n">
-        <v>65.196</v>
+        <v>65.30699999999999</v>
       </c>
       <c r="CC119" t="n">
-        <v>0.05128352561984081</v>
+        <v>0.1344990706287601</v>
       </c>
     </row>
     <row r="120">
@@ -29973,25 +29973,25 @@
         <v>0.0167384206540093</v>
       </c>
       <c r="BW120" t="n">
-        <v>2595</v>
+        <v>2592.5</v>
       </c>
       <c r="BX120" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY120" s="2" t="n">
         <v>44766.60072918981</v>
       </c>
       <c r="BZ120" t="n">
-        <v>20.106</v>
+        <v>20.103</v>
       </c>
       <c r="CA120" t="n">
-        <v>0.01341640786500056</v>
+        <v>0.01059349905471353</v>
       </c>
       <c r="CB120" t="n">
-        <v>49.01600000000001</v>
+        <v>49.12799999999999</v>
       </c>
       <c r="CC120" t="n">
-        <v>0.04827007354458918</v>
+        <v>0.1359575097022727</v>
       </c>
     </row>
     <row r="121">
@@ -30218,25 +30218,25 @@
         <v>0.00744676256274446</v>
       </c>
       <c r="BW121" t="n">
-        <v>2613</v>
+        <v>2610.5</v>
       </c>
       <c r="BX121" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY121" s="2" t="n">
         <v>44766.66322918981</v>
       </c>
       <c r="BZ121" t="n">
-        <v>20.096</v>
+        <v>20.088</v>
       </c>
       <c r="CA121" t="n">
-        <v>0.008944271910000358</v>
+        <v>0.01135292424395242</v>
       </c>
       <c r="CB121" t="n">
-        <v>32.678</v>
+        <v>32.77999999999999</v>
       </c>
       <c r="CC121" t="n">
-        <v>0.04764451699828634</v>
+        <v>0.1343296111973943</v>
       </c>
     </row>
     <row r="122">
@@ -30463,25 +30463,25 @@
         <v>0.000693365928851932</v>
       </c>
       <c r="BW122" t="n">
-        <v>2632</v>
+        <v>2629.5</v>
       </c>
       <c r="BX122" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY122" s="2" t="n">
         <v>44766.72920141204</v>
       </c>
       <c r="BZ122" t="n">
-        <v>20.092</v>
+        <v>20.091</v>
       </c>
       <c r="CA122" t="n">
-        <v>0.01095445115010401</v>
+        <v>0.007378647873725632</v>
       </c>
       <c r="CB122" t="n">
-        <v>14.594</v>
+        <v>14.679</v>
       </c>
       <c r="CC122" t="n">
-        <v>0.04560701700396536</v>
+        <v>0.1040779622313103</v>
       </c>
     </row>
     <row r="123">
@@ -30708,25 +30708,25 @@
         <v>0.000738172475947061</v>
       </c>
       <c r="BW123" t="n">
-        <v>2668</v>
+        <v>2665.5</v>
       </c>
       <c r="BX123" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY123" s="2" t="n">
         <v>44766.85420141204</v>
       </c>
       <c r="BZ123" t="n">
-        <v>29.854</v>
+        <v>29.819</v>
       </c>
       <c r="CA123" t="n">
-        <v>0.02302172886644312</v>
+        <v>0.04067486256208303</v>
       </c>
       <c r="CB123" t="n">
-        <v>14.422</v>
+        <v>14.482</v>
       </c>
       <c r="CC123" t="n">
-        <v>0.03346640106136268</v>
+        <v>0.07656515018088897</v>
       </c>
     </row>
     <row r="124">
@@ -30953,25 +30953,25 @@
         <v>0.00223596622001493</v>
       </c>
       <c r="BW124" t="n">
-        <v>2687</v>
+        <v>2684.5</v>
       </c>
       <c r="BX124" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY124" s="2" t="n">
         <v>44766.92017363426</v>
       </c>
       <c r="BZ124" t="n">
-        <v>30.07999999999999</v>
+        <v>30.07599999999999</v>
       </c>
       <c r="CA124" t="n">
-        <v>0</v>
+        <v>0.01264911064067443</v>
       </c>
       <c r="CB124" t="n">
-        <v>31.59</v>
+        <v>31.57</v>
       </c>
       <c r="CC124" t="n">
-        <v>0</v>
+        <v>0.02828427124746088</v>
       </c>
     </row>
     <row r="125">
@@ -31198,25 +31198,25 @@
         <v>0.00793594296504709</v>
       </c>
       <c r="BW125" t="n">
-        <v>2705</v>
+        <v>2702.5</v>
       </c>
       <c r="BX125" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY125" s="2" t="n">
         <v>44766.98267363426</v>
       </c>
       <c r="BZ125" t="n">
-        <v>30.11</v>
+        <v>30.11000000000001</v>
       </c>
       <c r="CA125" t="n">
-        <v>0.007071067811865533</v>
+        <v>0.004714045207910077</v>
       </c>
       <c r="CB125" t="n">
-        <v>47.47199999999999</v>
+        <v>47.42100000000001</v>
       </c>
       <c r="CC125" t="n">
-        <v>0.02489979919597656</v>
+        <v>0.06349978127696622</v>
       </c>
     </row>
     <row r="126">
@@ -31443,25 +31443,25 @@
         <v>0.007872515363269</v>
       </c>
       <c r="BW126" t="n">
-        <v>2723</v>
+        <v>2720.5</v>
       </c>
       <c r="BX126" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY126" s="2" t="n">
         <v>44767.04517363426</v>
       </c>
       <c r="BZ126" t="n">
-        <v>30.126</v>
+        <v>30.133</v>
       </c>
       <c r="CA126" t="n">
-        <v>0.005477225575050004</v>
+        <v>0.008232726023486799</v>
       </c>
       <c r="CB126" t="n">
-        <v>63.14</v>
+        <v>63.05999999999999</v>
       </c>
       <c r="CC126" t="n">
-        <v>0.04415880433164228</v>
+        <v>0.1006644591369469</v>
       </c>
     </row>
     <row r="127">
@@ -31688,25 +31688,25 @@
         <v>0.0146418399677523</v>
       </c>
       <c r="BW127" t="n">
-        <v>2742</v>
+        <v>2739.5</v>
       </c>
       <c r="BX127" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY127" s="2" t="n">
         <v>44767.11114585648</v>
       </c>
       <c r="BZ127" t="n">
-        <v>30.148</v>
+        <v>30.149</v>
       </c>
       <c r="CA127" t="n">
-        <v>0.01095445115010224</v>
+        <v>0.0119721899973786</v>
       </c>
       <c r="CB127" t="n">
-        <v>78.86800000000001</v>
+        <v>78.762</v>
       </c>
       <c r="CC127" t="n">
-        <v>0.06833739825308061</v>
+        <v>0.1326482399263424</v>
       </c>
     </row>
     <row r="128">
@@ -31933,25 +31933,25 @@
         <v>0.0101912022631151</v>
       </c>
       <c r="BW128" t="n">
-        <v>2778</v>
+        <v>2775.5</v>
       </c>
       <c r="BX128" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY128" s="2" t="n">
         <v>44767.23614585648</v>
       </c>
       <c r="BZ128" t="n">
-        <v>30.144</v>
+        <v>30.152</v>
       </c>
       <c r="CA128" t="n">
-        <v>0.008944271909999017</v>
+        <v>0.01475729574745219</v>
       </c>
       <c r="CB128" t="n">
-        <v>95.48999999999999</v>
+        <v>95.404</v>
       </c>
       <c r="CC128" t="n">
-        <v>0.04743416490252693</v>
+        <v>0.1078270219688247</v>
       </c>
     </row>
     <row r="129">
@@ -32178,25 +32178,25 @@
         <v>0.0102510500637109</v>
       </c>
       <c r="BW129" t="n">
-        <v>2797</v>
+        <v>2794.5</v>
       </c>
       <c r="BX129" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY129" s="2" t="n">
         <v>44767.3021180787</v>
       </c>
       <c r="BZ129" t="n">
-        <v>30.078</v>
+        <v>30.071</v>
       </c>
       <c r="CA129" t="n">
-        <v>0.01483239697419195</v>
+        <v>0.01286683937707909</v>
       </c>
       <c r="CB129" t="n">
-        <v>80.89599999999999</v>
+        <v>80.97</v>
       </c>
       <c r="CC129" t="n">
-        <v>0.05770615218501228</v>
+        <v>0.09451631252505088</v>
       </c>
     </row>
     <row r="130">
@@ -32423,25 +32423,25 @@
         <v>0.0100145233642166</v>
       </c>
       <c r="BW130" t="n">
-        <v>2815</v>
+        <v>2812.5</v>
       </c>
       <c r="BX130" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY130" s="2" t="n">
         <v>44767.3646180787</v>
       </c>
       <c r="BZ130" t="n">
-        <v>30.036</v>
+        <v>30.028</v>
       </c>
       <c r="CA130" t="n">
-        <v>0.01341640786499746</v>
+        <v>0.01813529401164609</v>
       </c>
       <c r="CB130" t="n">
-        <v>65.14000000000001</v>
+        <v>65.227</v>
       </c>
       <c r="CC130" t="n">
-        <v>0.02999999999999743</v>
+        <v>0.1071914175668976</v>
       </c>
     </row>
     <row r="131">
@@ -32668,25 +32668,25 @@
         <v>0.00775232271469488</v>
       </c>
       <c r="BW131" t="n">
-        <v>2834</v>
+        <v>2831.5</v>
       </c>
       <c r="BX131" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY131" s="2" t="n">
         <v>44767.43059030092</v>
       </c>
       <c r="BZ131" t="n">
-        <v>29.998</v>
+        <v>29.988</v>
       </c>
       <c r="CA131" t="n">
-        <v>0.01643167672515493</v>
+        <v>0.01751190071541861</v>
       </c>
       <c r="CB131" t="n">
-        <v>48.94</v>
+        <v>49.03</v>
       </c>
       <c r="CC131" t="n">
-        <v>0.04636809247747624</v>
+        <v>0.1092397973878267</v>
       </c>
     </row>
     <row r="132">
@@ -32913,10 +32913,10 @@
         <v>0.00429008930519794</v>
       </c>
       <c r="BW132" t="n">
-        <v>2852</v>
+        <v>2849.5</v>
       </c>
       <c r="BX132" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY132" s="2" t="n">
         <v>44767.49309030092</v>
@@ -32925,13 +32925,13 @@
         <v>29.978</v>
       </c>
       <c r="CA132" t="n">
-        <v>0.01095445115010353</v>
+        <v>0.01032795558988546</v>
       </c>
       <c r="CB132" t="n">
-        <v>32.556</v>
+        <v>32.638</v>
       </c>
       <c r="CC132" t="n">
-        <v>0.04159326868617304</v>
+        <v>0.09542885657214319</v>
       </c>
     </row>
     <row r="133">
@@ -33158,25 +33158,25 @@
         <v>0.000646252094560486</v>
       </c>
       <c r="BW133" t="n">
-        <v>2870</v>
+        <v>2867.5</v>
       </c>
       <c r="BX133" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY133" s="2" t="n">
         <v>44767.55559030092</v>
       </c>
       <c r="BZ133" t="n">
-        <v>29.978</v>
+        <v>29.972</v>
       </c>
       <c r="CA133" t="n">
-        <v>0.01095445115010224</v>
+        <v>0.01475729574745196</v>
       </c>
       <c r="CB133" t="n">
-        <v>14.586</v>
+        <v>14.649</v>
       </c>
       <c r="CC133" t="n">
-        <v>0.0450555213042759</v>
+        <v>0.08837420438114311</v>
       </c>
     </row>
     <row r="134">
@@ -33403,25 +33403,25 @@
         <v>0.000696523977819397</v>
       </c>
       <c r="BW134" t="n">
-        <v>2906</v>
+        <v>2903.5</v>
       </c>
       <c r="BX134" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY134" s="2" t="n">
         <v>44767.68059030092</v>
       </c>
       <c r="BZ134" t="n">
-        <v>39.912</v>
+        <v>39.84699999999999</v>
       </c>
       <c r="CA134" t="n">
-        <v>0.03898717737923939</v>
+        <v>0.08273787255879339</v>
       </c>
       <c r="CB134" t="n">
-        <v>14.482</v>
+        <v>14.535</v>
       </c>
       <c r="CC134" t="n">
-        <v>0.02489979919597745</v>
+        <v>0.06835365551470064</v>
       </c>
     </row>
     <row r="135">
@@ -33648,25 +33648,25 @@
         <v>0.00364646520416988</v>
       </c>
       <c r="BW135" t="n">
-        <v>2924</v>
+        <v>2921.5</v>
       </c>
       <c r="BX135" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY135" s="2" t="n">
         <v>44767.74309030092</v>
       </c>
       <c r="BZ135" t="n">
-        <v>40.09</v>
+        <v>40.09000000000001</v>
       </c>
       <c r="CA135" t="n">
         <v>0</v>
       </c>
       <c r="CB135" t="n">
-        <v>31.634</v>
+        <v>31.61199999999999</v>
       </c>
       <c r="CC135" t="n">
-        <v>0.01341640786499949</v>
+        <v>0.03084008934992382</v>
       </c>
     </row>
     <row r="136">
@@ -33893,25 +33893,25 @@
         <v>0.0101244929214858</v>
       </c>
       <c r="BW136" t="n">
-        <v>2943</v>
+        <v>2940.5</v>
       </c>
       <c r="BX136" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY136" s="2" t="n">
         <v>44767.80906252315</v>
       </c>
       <c r="BZ136" t="n">
-        <v>40.13</v>
+        <v>40.133</v>
       </c>
       <c r="CA136" t="n">
-        <v>0</v>
+        <v>0.009486832980503491</v>
       </c>
       <c r="CB136" t="n">
-        <v>47.526</v>
+        <v>47.47799999999999</v>
       </c>
       <c r="CC136" t="n">
-        <v>0.02190890230020707</v>
+        <v>0.0654556677793757</v>
       </c>
     </row>
     <row r="137">
@@ -34138,25 +34138,25 @@
         <v>0.0147341222341297</v>
       </c>
       <c r="BW137" t="n">
-        <v>2961</v>
+        <v>2958.5</v>
       </c>
       <c r="BX137" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY137" s="2" t="n">
         <v>44767.87156252315</v>
       </c>
       <c r="BZ137" t="n">
-        <v>40.184</v>
+        <v>40.202</v>
       </c>
       <c r="CA137" t="n">
-        <v>0.02701851217221121</v>
+        <v>0.02740640638812471</v>
       </c>
       <c r="CB137" t="n">
-        <v>63.21</v>
+        <v>63.141</v>
       </c>
       <c r="CC137" t="n">
-        <v>0.03674234614174961</v>
+        <v>0.08723531395025585</v>
       </c>
     </row>
     <row r="138">
@@ -34383,25 +34383,25 @@
         <v>0.0127648855738276</v>
       </c>
       <c r="BW138" t="n">
-        <v>2979</v>
+        <v>2976.5</v>
       </c>
       <c r="BX138" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY138" s="2" t="n">
         <v>44767.93406252315</v>
       </c>
       <c r="BZ138" t="n">
-        <v>40.23</v>
+        <v>40.24</v>
       </c>
       <c r="CA138" t="n">
-        <v>0</v>
+        <v>0.01054092553389727</v>
       </c>
       <c r="CB138" t="n">
-        <v>78.952</v>
+        <v>78.84100000000001</v>
       </c>
       <c r="CC138" t="n">
-        <v>0.06220932405998312</v>
+        <v>0.1354375624903737</v>
       </c>
     </row>
     <row r="139">
@@ -34628,25 +34628,25 @@
         <v>0.0100066671588096</v>
       </c>
       <c r="BW139" t="n">
-        <v>3015</v>
+        <v>3012.5</v>
       </c>
       <c r="BX139" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY139" s="2" t="n">
         <v>44768.05906252315</v>
       </c>
       <c r="BZ139" t="n">
-        <v>40.23399999999999</v>
+        <v>40.24</v>
       </c>
       <c r="CA139" t="n">
-        <v>0.00894427191000112</v>
+        <v>0.01054092553389658</v>
       </c>
       <c r="CB139" t="n">
-        <v>95.78800000000001</v>
+        <v>95.68299999999999</v>
       </c>
       <c r="CC139" t="n">
-        <v>0.07328028384223985</v>
+        <v>0.1271088772142517</v>
       </c>
     </row>
     <row r="140">
@@ -34873,25 +34873,25 @@
         <v>0.0143549049531653</v>
       </c>
       <c r="BW140" t="n">
-        <v>3034</v>
+        <v>3031.5</v>
       </c>
       <c r="BX140" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY140" s="2" t="n">
         <v>44768.12503474537</v>
       </c>
       <c r="BZ140" t="n">
-        <v>40.096</v>
+        <v>40.08900000000001</v>
       </c>
       <c r="CA140" t="n">
-        <v>0.01341640786499567</v>
+        <v>0.01370320319406095</v>
       </c>
       <c r="CB140" t="n">
-        <v>80.98800000000001</v>
+        <v>81.04999999999998</v>
       </c>
       <c r="CC140" t="n">
-        <v>0.04868264577855789</v>
+        <v>0.08445906306213793</v>
       </c>
     </row>
     <row r="141">
@@ -35118,25 +35118,25 @@
         <v>0.00942179549543278</v>
       </c>
       <c r="BW141" t="n">
-        <v>3052</v>
+        <v>3049.5</v>
       </c>
       <c r="BX141" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY141" s="2" t="n">
         <v>44768.18753474537</v>
       </c>
       <c r="BZ141" t="n">
-        <v>40.07</v>
+        <v>40.057</v>
       </c>
       <c r="CA141" t="n">
-        <v>0</v>
+        <v>0.0141813649241198</v>
       </c>
       <c r="CB141" t="n">
-        <v>65.06999999999999</v>
+        <v>65.178</v>
       </c>
       <c r="CC141" t="n">
-        <v>0.05873670062235437</v>
+        <v>0.1303670033235265</v>
       </c>
     </row>
     <row r="142">
@@ -35363,25 +35363,25 @@
         <v>0.00428845870951982</v>
       </c>
       <c r="BW142" t="n">
-        <v>3070</v>
+        <v>3067.5</v>
       </c>
       <c r="BX142" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY142" s="2" t="n">
         <v>44768.25003474537</v>
       </c>
       <c r="BZ142" t="n">
-        <v>40.028</v>
+        <v>40.021</v>
       </c>
       <c r="CA142" t="n">
-        <v>0.02049390153191706</v>
+        <v>0.01595131481867242</v>
       </c>
       <c r="CB142" t="n">
-        <v>48.914</v>
+        <v>49.001</v>
       </c>
       <c r="CC142" t="n">
-        <v>0.04722287581246848</v>
+        <v>0.1053512642965864</v>
       </c>
     </row>
     <row r="143">
@@ -35608,25 +35608,25 @@
         <v>0.00334732089469035</v>
       </c>
       <c r="BW143" t="n">
-        <v>3089</v>
+        <v>3086.5</v>
       </c>
       <c r="BX143" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY143" s="2" t="n">
         <v>44768.31600696759</v>
       </c>
       <c r="BZ143" t="n">
-        <v>40.01</v>
+        <v>40.002</v>
       </c>
       <c r="CA143" t="n">
-        <v>0</v>
+        <v>0.01032795558988455</v>
       </c>
       <c r="CB143" t="n">
-        <v>32.424</v>
+        <v>32.492</v>
       </c>
       <c r="CC143" t="n">
-        <v>0.04560701700396357</v>
+        <v>0.08651268372004943</v>
       </c>
     </row>
     <row r="144">
@@ -35853,25 +35853,25 @@
         <v>0.000609540380752488</v>
       </c>
       <c r="BW144" t="n">
-        <v>3107</v>
+        <v>3104.5</v>
       </c>
       <c r="BX144" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY144" s="2" t="n">
         <v>44768.37850696759</v>
       </c>
       <c r="BZ144" t="n">
-        <v>40.00599999999999</v>
+        <v>40.001</v>
       </c>
       <c r="CA144" t="n">
-        <v>0.008944271909998804</v>
+        <v>0.008755950357706776</v>
       </c>
       <c r="CB144" t="n">
-        <v>14.58</v>
+        <v>14.655</v>
       </c>
       <c r="CC144" t="n">
-        <v>0.02738612787525814</v>
+        <v>0.08746427842267997</v>
       </c>
     </row>
     <row r="145">
@@ -36098,19 +36098,19 @@
         <v>0.000481116353997318</v>
       </c>
       <c r="BW145" t="n">
-        <v>3179</v>
+        <v>3176.5</v>
       </c>
       <c r="BX145" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY145" s="2" t="n">
         <v>44768.62850696759</v>
       </c>
       <c r="BZ145" t="n">
-        <v>30.066</v>
+        <v>30.064</v>
       </c>
       <c r="CA145" t="n">
-        <v>0.01140175425099103</v>
+        <v>0.01173787790777162</v>
       </c>
       <c r="CB145" t="n">
         <v>13.92</v>
@@ -36343,25 +36343,25 @@
         <v>0.00378287070925243</v>
       </c>
       <c r="BW146" t="n">
-        <v>3198</v>
+        <v>3195.5</v>
       </c>
       <c r="BX146" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY146" s="2" t="n">
         <v>44768.69447918981</v>
       </c>
       <c r="BZ146" t="n">
-        <v>30.102</v>
+        <v>30.107</v>
       </c>
       <c r="CA146" t="n">
-        <v>0.01303840481040549</v>
+        <v>0.01059349905471399</v>
       </c>
       <c r="CB146" t="n">
-        <v>31.038</v>
+        <v>30.99</v>
       </c>
       <c r="CC146" t="n">
-        <v>0.03346640106136392</v>
+        <v>0.05962847939999466</v>
       </c>
     </row>
     <row r="147">
@@ -36588,25 +36588,25 @@
         <v>0.00463016858749802</v>
       </c>
       <c r="BW147" t="n">
-        <v>3216</v>
+        <v>3213.5</v>
       </c>
       <c r="BX147" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY147" s="2" t="n">
         <v>44768.75697918981</v>
       </c>
       <c r="BZ147" t="n">
-        <v>30.118</v>
+        <v>30.122</v>
       </c>
       <c r="CA147" t="n">
-        <v>0.00447213595500056</v>
+        <v>0.006324555320336283</v>
       </c>
       <c r="CB147" t="n">
-        <v>46.948</v>
+        <v>46.88000000000001</v>
       </c>
       <c r="CC147" t="n">
-        <v>0.03193743884534481</v>
+        <v>0.08246211251235068</v>
       </c>
     </row>
     <row r="148">
@@ -36833,25 +36833,25 @@
         <v>0.0106159405379435</v>
       </c>
       <c r="BW148" t="n">
-        <v>3235</v>
+        <v>3232.5</v>
       </c>
       <c r="BX148" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY148" s="2" t="n">
         <v>44768.82295141204</v>
       </c>
       <c r="BZ148" t="n">
-        <v>30.138</v>
+        <v>30.141</v>
       </c>
       <c r="CA148" t="n">
-        <v>0.004472135955000676</v>
+        <v>0.007378647873725908</v>
       </c>
       <c r="CB148" t="n">
-        <v>62.862</v>
+        <v>62.787</v>
       </c>
       <c r="CC148" t="n">
-        <v>0.0268328157299985</v>
+        <v>0.09428679653058303</v>
       </c>
     </row>
     <row r="149">
@@ -37078,25 +37078,25 @@
         <v>0.00898283228787103</v>
       </c>
       <c r="BW149" t="n">
-        <v>3253</v>
+        <v>3250.5</v>
       </c>
       <c r="BX149" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY149" s="2" t="n">
         <v>44768.88545141204</v>
       </c>
       <c r="BZ149" t="n">
-        <v>30.146</v>
+        <v>30.153</v>
       </c>
       <c r="CA149" t="n">
-        <v>0.008944271909998455</v>
+        <v>0.01251665557034568</v>
       </c>
       <c r="CB149" t="n">
-        <v>78.792</v>
+        <v>78.66799999999999</v>
       </c>
       <c r="CC149" t="n">
-        <v>0.05718391382198855</v>
+        <v>0.1503181810545782</v>
       </c>
     </row>
     <row r="150">
@@ -37323,25 +37323,25 @@
         <v>0.00448269633309252</v>
       </c>
       <c r="BW150" t="n">
-        <v>3290</v>
+        <v>3287.5</v>
       </c>
       <c r="BX150" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY150" s="2" t="n">
         <v>44769.01392363426</v>
       </c>
       <c r="BZ150" t="n">
-        <v>30.154</v>
+        <v>30.15500000000001</v>
       </c>
       <c r="CA150" t="n">
-        <v>0.01341640786499847</v>
+        <v>0.01354006400772674</v>
       </c>
       <c r="CB150" t="n">
-        <v>95.60799999999999</v>
+        <v>95.529</v>
       </c>
       <c r="CC150" t="n">
-        <v>0.04438468204234355</v>
+        <v>0.09677580046456311</v>
       </c>
     </row>
     <row r="151">
@@ -37568,25 +37568,25 @@
         <v>0.0105970049357667</v>
       </c>
       <c r="BW151" t="n">
-        <v>3308</v>
+        <v>3305.5</v>
       </c>
       <c r="BX151" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY151" s="2" t="n">
         <v>44769.07642363426</v>
       </c>
       <c r="BZ151" t="n">
-        <v>30.07399999999999</v>
+        <v>30.066</v>
       </c>
       <c r="CA151" t="n">
-        <v>0.01516575088810398</v>
+        <v>0.01349897115421231</v>
       </c>
       <c r="CB151" t="n">
-        <v>81.01600000000001</v>
+        <v>81.10600000000001</v>
       </c>
       <c r="CC151" t="n">
-        <v>0.04159326868617666</v>
+        <v>0.1095647956436907</v>
       </c>
     </row>
     <row r="152">
@@ -37813,25 +37813,25 @@
         <v>0.0047073229863572</v>
       </c>
       <c r="BW152" t="n">
-        <v>3326</v>
+        <v>3323.5</v>
       </c>
       <c r="BX152" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY152" s="2" t="n">
         <v>44769.13892363426</v>
       </c>
       <c r="BZ152" t="n">
-        <v>30.046</v>
+        <v>30.029</v>
       </c>
       <c r="CA152" t="n">
-        <v>0.01949358868961896</v>
+        <v>0.02378141197564785</v>
       </c>
       <c r="CB152" t="n">
-        <v>65.116</v>
+        <v>65.21799999999999</v>
       </c>
       <c r="CC152" t="n">
-        <v>0.07765307463327165</v>
+        <v>0.1310470653365944</v>
       </c>
     </row>
     <row r="153">
@@ -38058,25 +38058,25 @@
         <v>0.00553504713217753</v>
       </c>
       <c r="BW153" t="n">
-        <v>3344</v>
+        <v>3341.5</v>
       </c>
       <c r="BX153" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY153" s="2" t="n">
         <v>44769.20142363426</v>
       </c>
       <c r="BZ153" t="n">
-        <v>30</v>
+        <v>29.989</v>
       </c>
       <c r="CA153" t="n">
-        <v>0.007071067811867208</v>
+        <v>0.01449137674619124</v>
       </c>
       <c r="CB153" t="n">
-        <v>48.808</v>
+        <v>48.92</v>
       </c>
       <c r="CC153" t="n">
-        <v>0.04658325879540882</v>
+        <v>0.1354826762193412</v>
       </c>
     </row>
     <row r="154">
@@ -38303,25 +38303,25 @@
         <v>0.00204780108581577</v>
       </c>
       <c r="BW154" t="n">
-        <v>3362</v>
+        <v>3359.5</v>
       </c>
       <c r="BX154" t="n">
-        <v>1.58113883008419</v>
+        <v>3.027650354097492</v>
       </c>
       <c r="BY154" s="2" t="n">
         <v>44769.26392363426</v>
       </c>
       <c r="BZ154" t="n">
-        <v>29.966</v>
+        <v>29.967</v>
       </c>
       <c r="CA154" t="n">
-        <v>0.008944271909997529</v>
+        <v>0.01159501808728471</v>
       </c>
       <c r="CB154" t="n">
-        <v>32.412</v>
+        <v>32.499</v>
       </c>
       <c r="CC154" t="n">
-        <v>0.02949576240750959</v>
+        <v>0.1070254383053111</v>
       </c>
     </row>
     <row r="155">

</xml_diff>